<commit_message>
More notes for the Crawler.
</commit_message>
<xml_diff>
--- a/Notes/table_fetch_runner_locations.xlsx
+++ b/Notes/table_fetch_runner_locations.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="157">
   <si>
     <t>Type de course</t>
   </si>
@@ -498,13 +498,19 @@
   </si>
   <si>
     <t>h3.clearfix, Séparé par ', ' : 4è élmt</t>
+  </si>
+  <si>
+    <t>Pris ici</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -524,6 +530,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1" tint="0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -601,7 +615,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -617,12 +631,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -659,9 +667,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -682,9 +687,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -705,10 +707,61 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1441,7 +1494,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="D47" s="4" t="s">
         <v>30</v>
       </c>
@@ -2530,1227 +2583,1344 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C38" sqref="A38:XFD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.140625" style="15" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" style="16" customWidth="1"/>
-    <col min="5" max="5" width="36.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="41.140625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" style="14" customWidth="1"/>
+    <col min="6" max="6" width="36.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.42578125" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="7"/>
-      <c r="C2" s="9" t="s">
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="E2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="F2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="G2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="H2" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="I2" s="12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="34" t="s">
         <v>119</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="E3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="F3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="G3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="H3" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="I3" s="18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="34"/>
       <c r="B4" t="s">
         <v>120</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="E4" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="F4" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="G4" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="H4" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="H4" s="20" t="s">
+      <c r="I4" s="18" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="34"/>
       <c r="B5" t="s">
         <v>122</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="E5" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="F5" s="15" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="34"/>
       <c r="B6" t="s">
         <v>124</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="C6" t="s">
+        <v>156</v>
+      </c>
+      <c r="F6" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="G6" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="H6" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="H6" s="20" t="s">
+      <c r="I6" s="18" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="34"/>
       <c r="B7" t="s">
         <v>82</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" t="s">
+        <v>156</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="E7" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="F7" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="G7" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="H7" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="I7" s="18" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="34"/>
       <c r="B8" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="E8" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="F8" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="G8" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="H8" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="I8" s="18" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="34"/>
       <c r="B9" t="s">
         <v>130</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" t="s">
+        <v>156</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="E9" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="F9" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="G9" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="H9" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="I9" s="18" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="34"/>
       <c r="B10" t="s">
         <v>133</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" t="s">
+        <v>156</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="E10" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="F10" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="G10" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="H10" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="H10" s="20" t="s">
+      <c r="I10" s="18" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" t="s">
+    <row r="11" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="34"/>
+      <c r="B11" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="D11" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="E11" s="40" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="44"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="34"/>
       <c r="B12" t="s">
         <v>136</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" t="s">
+        <v>156</v>
+      </c>
+      <c r="D12" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="E12" s="14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="34"/>
       <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D13" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="E13" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="F13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="G13" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="H13" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="20" t="s">
+      <c r="I13" s="18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" t="s">
+    <row r="14" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="34"/>
+      <c r="B14" s="38" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" t="s">
+      <c r="D14" s="39"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="44"/>
+    </row>
+    <row r="15" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="34"/>
+      <c r="B15" s="38" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="44"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="34"/>
       <c r="B16" t="s">
         <v>139</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="C16" t="s">
+        <v>156</v>
+      </c>
+      <c r="F16" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="G16" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="G16" s="19" t="s">
+      <c r="H16" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="H16" s="20" t="s">
+      <c r="I16" s="18" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="34"/>
       <c r="B17" t="s">
         <v>142</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="C17" t="s">
+        <v>156</v>
+      </c>
+      <c r="F17" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="F17" s="18" t="s">
+      <c r="G17" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="G17" s="19" t="s">
+      <c r="H17" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="H17" s="20" t="s">
+      <c r="I17" s="18" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="34"/>
       <c r="B18" t="s">
         <v>145</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="C18" t="s">
+        <v>156</v>
+      </c>
+      <c r="G18" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="G18" s="19" t="s">
+      <c r="H18" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="H18" s="20" t="s">
+      <c r="I18" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="34"/>
       <c r="B19" t="s">
         <v>146</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" t="s">
+        <v>156</v>
+      </c>
+      <c r="D19" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="E19" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="F19" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="F19" s="18" t="s">
+      <c r="G19" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="G19" s="19" t="s">
+      <c r="H19" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="H19" s="20" t="s">
+      <c r="I19" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="34"/>
       <c r="B20" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" t="s">
+        <v>156</v>
+      </c>
+      <c r="D20" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="E20" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="F20" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="G20" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G20" s="19" t="s">
+      <c r="H20" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="H20" s="20" t="s">
+      <c r="I20" s="18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="34"/>
       <c r="B21" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" t="s">
+        <v>156</v>
+      </c>
+      <c r="D21" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="E21" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E21" s="17" t="s">
+      <c r="F21" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="F21" s="18" t="s">
+      <c r="G21" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="G21" s="19" t="s">
+      <c r="H21" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="H21" s="20" t="s">
+      <c r="I21" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="34"/>
       <c r="B22" t="s">
         <v>76</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" t="s">
+        <v>156</v>
+      </c>
+      <c r="D22" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="E22" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="F22" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="F22" s="18" t="s">
+      <c r="G22" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="G22" s="19" t="s">
+      <c r="H22" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="H22" s="20" t="s">
+      <c r="I22" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="21" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="36" t="s">
         <v>147</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="D23" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="D23" s="24" t="s">
+      <c r="E23" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="E23" s="25" t="s">
+      <c r="F23" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="F23" s="26" t="s">
+      <c r="G23" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="G23" s="27" t="s">
+      <c r="H23" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="H23" s="28" t="s">
+      <c r="I23" s="25" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
-      <c r="B24" s="30" t="s">
+    <row r="24" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="37"/>
+      <c r="B24" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="31" t="s">
+      <c r="C24" s="45"/>
+      <c r="D24" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="32" t="s">
+      <c r="E24" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="33" t="s">
+      <c r="F24" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="34" t="s">
+      <c r="G24" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="G24" s="35" t="s">
+      <c r="H24" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="H24" s="36" t="s">
+      <c r="I24" s="51" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="29"/>
-      <c r="B25" s="30" t="s">
+    <row r="25" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="37"/>
+      <c r="B25" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="C25" s="31" t="s">
+      <c r="C25" s="45"/>
+      <c r="D25" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="D25" s="32" t="s">
+      <c r="E25" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="E25" s="33" t="s">
+      <c r="F25" s="48" t="s">
         <v>121</v>
       </c>
-      <c r="F25" s="34" t="s">
+      <c r="G25" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="G25" s="35" t="s">
+      <c r="H25" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="H25" s="36" t="s">
+      <c r="I25" s="51" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="29"/>
-      <c r="B26" s="30" t="s">
+    <row r="26" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="37"/>
+      <c r="B26" s="45" t="s">
         <v>122</v>
       </c>
-      <c r="C26" s="31" t="s">
+      <c r="C26" s="45"/>
+      <c r="D26" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="D26" s="32" t="s">
+      <c r="E26" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="E26" s="33"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="36"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
-      <c r="B27" s="30" t="s">
+      <c r="F26" s="48"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="51"/>
+    </row>
+    <row r="27" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="37"/>
+      <c r="B27" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="C27" s="31"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="33" t="s">
+      <c r="C27" s="45"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="48" t="s">
         <v>125</v>
       </c>
-      <c r="F27" s="34" t="s">
+      <c r="G27" s="49" t="s">
         <v>125</v>
       </c>
-      <c r="G27" s="35" t="s">
+      <c r="H27" s="50" t="s">
         <v>125</v>
       </c>
-      <c r="H27" s="36" t="s">
+      <c r="I27" s="51" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
-      <c r="B28" s="30" t="s">
+    <row r="28" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="37"/>
+      <c r="B28" s="45" t="s">
         <v>130</v>
       </c>
-      <c r="C28" s="31" t="s">
+      <c r="C28" s="45"/>
+      <c r="D28" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="32" t="s">
+      <c r="E28" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="E28" s="33" t="s">
+      <c r="F28" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="F28" s="34" t="s">
+      <c r="G28" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="G28" s="35" t="s">
+      <c r="H28" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="H28" s="36" t="s">
+      <c r="I28" s="51" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
-      <c r="B29" s="30" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="37"/>
+      <c r="B29" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="31" t="s">
+      <c r="C29" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="D29" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="D29" s="32" t="s">
+      <c r="E29" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="E29" s="33"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="36"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
-      <c r="B30" s="30" t="s">
+      <c r="F29" s="29"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="32"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="37"/>
+      <c r="B30" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="C30" s="31" t="s">
+      <c r="C30" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="D30" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="D30" s="32" t="s">
+      <c r="E30" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="E30" s="33" t="s">
+      <c r="F30" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="F30" s="34" t="s">
+      <c r="G30" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="G30" s="35" t="s">
+      <c r="H30" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="H30" s="36" t="s">
+      <c r="I30" s="32" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="29"/>
-      <c r="B31" s="30" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="37"/>
+      <c r="B31" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="C31" s="31" t="s">
+      <c r="C31" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="D31" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="D31" s="32" t="s">
+      <c r="E31" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="E31" s="33" t="s">
+      <c r="F31" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="F31" s="34" t="s">
+      <c r="G31" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="G31" s="35" t="s">
+      <c r="H31" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="H31" s="36" t="s">
+      <c r="I31" s="32" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="29"/>
-      <c r="B32" s="30" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="37"/>
+      <c r="B32" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="31" t="s">
+      <c r="C32" s="53" t="s">
+        <v>156</v>
+      </c>
+      <c r="D32" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="D32" s="32" t="s">
+      <c r="E32" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="E32" s="33" t="s">
+      <c r="F32" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="F32" s="34" t="s">
+      <c r="G32" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="G32" s="35" t="s">
+      <c r="H32" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="H32" s="36" t="s">
+      <c r="I32" s="32" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="29"/>
-      <c r="B33" s="30" t="s">
+    <row r="33" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="37"/>
+      <c r="B33" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="C33" s="31" t="s">
+      <c r="C33" s="45"/>
+      <c r="D33" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="D33" s="32" t="s">
+      <c r="E33" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="E33" s="33" t="s">
+      <c r="F33" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="F33" s="34" t="s">
+      <c r="G33" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="G33" s="35" t="s">
+      <c r="H33" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="H33" s="36" t="s">
+      <c r="I33" s="51" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="29"/>
-      <c r="B34" s="30" t="s">
+    <row r="34" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="37"/>
+      <c r="B34" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="31" t="s">
+      <c r="C34" s="45"/>
+      <c r="D34" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="D34" s="32" t="s">
+      <c r="E34" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="E34" s="33" t="s">
+      <c r="F34" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="F34" s="34" t="s">
+      <c r="G34" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="G34" s="35" t="s">
+      <c r="H34" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="H34" s="36" t="s">
+      <c r="I34" s="51" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="29"/>
-      <c r="B35" s="30" t="s">
+    <row r="35" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="37"/>
+      <c r="B35" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="C35" s="31" t="s">
+      <c r="C35" s="45"/>
+      <c r="D35" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="D35" s="32" t="s">
+      <c r="E35" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="E35" s="33" t="s">
+      <c r="F35" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="F35" s="34" t="s">
+      <c r="G35" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="G35" s="35" t="s">
+      <c r="H35" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="H35" s="36" t="s">
+      <c r="I35" s="51" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="29"/>
-      <c r="B36" s="37" t="s">
+    <row r="36" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="37"/>
+      <c r="B36" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="C36" s="31" t="s">
+      <c r="C36" s="52"/>
+      <c r="D36" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="D36" s="32" t="s">
+      <c r="E36" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="E36" s="33" t="s">
+      <c r="F36" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="F36" s="34" t="s">
+      <c r="G36" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="G36" s="35" t="s">
+      <c r="H36" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="H36" s="36" t="s">
+      <c r="I36" s="51" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="21" t="s">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="36" t="s">
         <v>149</v>
       </c>
-      <c r="B37" s="38" t="s">
+      <c r="B37" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="C37" s="23" t="s">
+      <c r="C37" s="33"/>
+      <c r="D37" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="D37" s="24" t="s">
+      <c r="E37" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="E37" s="25" t="s">
+      <c r="F37" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="F37" s="26" t="s">
+      <c r="G37" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="G37" s="27" t="s">
+      <c r="H37" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="H37" s="36" t="s">
+      <c r="I37" s="32" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="29"/>
-      <c r="B38" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="C38" s="31" t="s">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="37"/>
+      <c r="B38" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38" s="26"/>
+      <c r="D38" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="D38" s="32" t="s">
+      <c r="E38" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="E38" s="33" t="s">
+      <c r="F38" s="29" t="s">
         <v>150</v>
       </c>
-      <c r="F38" s="34" t="s">
+      <c r="G38" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="G38" s="35" t="s">
+      <c r="H38" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="H38" s="36" t="s">
+      <c r="I38" s="32" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="29"/>
-      <c r="B39" s="30" t="s">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="37"/>
+      <c r="B39" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="C39" s="31" t="s">
+      <c r="C39" s="26"/>
+      <c r="D39" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="D39" s="32" t="s">
+      <c r="E39" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="E39" s="33" t="s">
+      <c r="F39" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="F39" s="34" t="s">
+      <c r="G39" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="G39" s="35" t="s">
+      <c r="H39" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="H39" s="36" t="s">
+      <c r="I39" s="32" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="29"/>
-      <c r="B40" s="30" t="s">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="37"/>
+      <c r="B40" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="C40" s="31" t="s">
+      <c r="C40" s="26"/>
+      <c r="D40" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="D40" s="32" t="s">
+      <c r="E40" s="28" t="s">
         <v>152</v>
       </c>
-      <c r="E40" s="33" t="s">
+      <c r="F40" s="29" t="s">
         <v>152</v>
       </c>
-      <c r="F40" s="34" t="s">
+      <c r="G40" s="30" t="s">
         <v>152</v>
       </c>
-      <c r="G40" s="35" t="s">
+      <c r="H40" s="31" t="s">
         <v>152</v>
       </c>
-      <c r="H40" s="36" t="s">
+      <c r="I40" s="32" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="29"/>
-      <c r="B41" s="30" t="s">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="37"/>
+      <c r="B41" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="C41" s="31" t="s">
+      <c r="C41" s="26"/>
+      <c r="D41" s="27" t="s">
         <v>153</v>
       </c>
-      <c r="D41" s="32" t="s">
+      <c r="E41" s="28" t="s">
         <v>153</v>
       </c>
-      <c r="E41" s="33" t="s">
+      <c r="F41" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="F41" s="34" t="s">
+      <c r="G41" s="30" t="s">
         <v>153</v>
       </c>
-      <c r="G41" s="35" t="s">
+      <c r="H41" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="H41" s="36" t="s">
+      <c r="I41" s="32" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="29"/>
-      <c r="B42" s="30" t="s">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="37"/>
+      <c r="B42" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="C42" s="31" t="s">
+      <c r="C42" s="26"/>
+      <c r="D42" s="27" t="s">
         <v>154</v>
       </c>
-      <c r="D42" s="32" t="s">
+      <c r="E42" s="28" t="s">
         <v>154</v>
       </c>
-      <c r="E42" s="33" t="s">
+      <c r="F42" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="F42" s="34" t="s">
+      <c r="G42" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="G42" s="35" t="s">
+      <c r="H42" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="H42" s="36" t="s">
+      <c r="I42" s="32" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="29"/>
-      <c r="B43" s="30" t="s">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="37"/>
+      <c r="B43" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="C43" s="31" t="s">
+      <c r="C43" s="26"/>
+      <c r="D43" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="D43" s="32" t="s">
+      <c r="E43" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="E43" s="33" t="s">
+      <c r="F43" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="F43" s="34" t="s">
+      <c r="G43" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="G43" s="35" t="s">
+      <c r="H43" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="H43" s="36" t="s">
+      <c r="I43" s="32" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="29"/>
-      <c r="B44" s="30" t="s">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="37"/>
+      <c r="B44" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="C44" s="31" t="s">
+      <c r="C44" s="26"/>
+      <c r="D44" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="D44" s="32" t="s">
+      <c r="E44" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="E44" s="33" t="s">
+      <c r="F44" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="F44" s="34" t="s">
+      <c r="G44" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="G44" s="35" t="s">
+      <c r="H44" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="H44" s="36" t="s">
+      <c r="I44" s="32" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="29"/>
-      <c r="B45" s="30" t="s">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="37"/>
+      <c r="B45" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="C45" s="31" t="s">
+      <c r="C45" s="26"/>
+      <c r="D45" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="D45" s="32" t="s">
+      <c r="E45" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="E45" s="33" t="s">
+      <c r="F45" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="F45" s="34" t="s">
+      <c r="G45" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="G45" s="35" t="s">
+      <c r="H45" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="H45" s="36" t="s">
+      <c r="I45" s="32" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="29"/>
-      <c r="B46" s="30" t="s">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="37"/>
+      <c r="B46" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="C46" s="31" t="s">
+      <c r="C46" s="26"/>
+      <c r="D46" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="D46" s="32" t="s">
+      <c r="E46" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="E46" s="33" t="s">
+      <c r="F46" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="F46" s="34" t="s">
+      <c r="G46" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="G46" s="35" t="s">
+      <c r="H46" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="H46" s="36" t="s">
+      <c r="I46" s="32" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="29"/>
-      <c r="B47" s="30" t="s">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="37"/>
+      <c r="B47" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C47" s="31" t="s">
+      <c r="C47" s="26"/>
+      <c r="D47" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="D47" s="32" t="s">
+      <c r="E47" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="E47" s="33" t="s">
+      <c r="F47" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="F47" s="34" t="s">
+      <c r="G47" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="G47" s="35" t="s">
+      <c r="H47" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="H47" s="36" t="s">
+      <c r="I47" s="32" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="29"/>
-      <c r="B48" s="30" t="s">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="37"/>
+      <c r="B48" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C48" s="31" t="s">
+      <c r="C48" s="26"/>
+      <c r="D48" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="D48" s="32" t="s">
+      <c r="E48" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="E48" s="33" t="s">
+      <c r="F48" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="F48" s="34" t="s">
+      <c r="G48" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="G48" s="35" t="s">
+      <c r="H48" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="H48" s="36" t="s">
+      <c r="I48" s="32" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="29"/>
-      <c r="B49" s="30" t="s">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="37"/>
+      <c r="B49" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C49" s="31" t="s">
+      <c r="C49" s="26"/>
+      <c r="D49" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="D49" s="32" t="s">
+      <c r="E49" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="E49" s="33" t="s">
+      <c r="F49" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="F49" s="34" t="s">
+      <c r="G49" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="G49" s="35" t="s">
+      <c r="H49" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="H49" s="36" t="s">
+      <c r="I49" s="32" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="29"/>
-      <c r="B50" s="30" t="s">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="37"/>
+      <c r="B50" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="C50" s="31" t="s">
+      <c r="C50" s="26"/>
+      <c r="D50" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="D50" s="32" t="s">
+      <c r="E50" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="E50" s="33" t="s">
+      <c r="F50" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="F50" s="34" t="s">
+      <c r="G50" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="G50" s="35" t="s">
+      <c r="H50" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="H50" s="36" t="s">
+      <c r="I50" s="32" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="29"/>
-      <c r="B51" s="30" t="s">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="37"/>
+      <c r="B51" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="C51" s="31" t="s">
+      <c r="C51" s="26"/>
+      <c r="D51" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="D51" s="32" t="s">
+      <c r="E51" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="E51" s="33" t="s">
+      <c r="F51" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="F51" s="34" t="s">
+      <c r="G51" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="G51" s="35" t="s">
+      <c r="H51" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="H51" s="36" t="s">
+      <c r="I51" s="32" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="29"/>
-      <c r="B52" s="30" t="s">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="37"/>
+      <c r="B52" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="C52" s="31" t="s">
+      <c r="C52" s="26"/>
+      <c r="D52" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="D52" s="32" t="s">
+      <c r="E52" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="E52" s="33" t="s">
+      <c r="F52" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="F52" s="34" t="s">
+      <c r="G52" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="G52" s="35" t="s">
+      <c r="H52" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="H52" s="36" t="s">
+      <c r="I52" s="32" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="29"/>
-      <c r="B53" s="30" t="s">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="37"/>
+      <c r="B53" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="C53" s="31" t="s">
+      <c r="C53" s="26"/>
+      <c r="D53" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="D53" s="32" t="s">
+      <c r="E53" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="E53" s="33" t="s">
+      <c r="F53" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="F53" s="34" t="s">
+      <c r="G53" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="G53" s="35" t="s">
+      <c r="H53" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="H53" s="36" t="s">
+      <c r="I53" s="32" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="29"/>
-      <c r="B54" s="30" t="s">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="37"/>
+      <c r="B54" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="C54" s="31" t="s">
+      <c r="C54" s="26"/>
+      <c r="D54" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="D54" s="32" t="s">
+      <c r="E54" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="E54" s="33" t="s">
+      <c r="F54" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="F54" s="34" t="s">
+      <c r="G54" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="G54" s="35" t="s">
+      <c r="H54" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="H54" s="36" t="s">
+      <c r="I54" s="32" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="29"/>
-      <c r="B55" s="30" t="s">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="37"/>
+      <c r="B55" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="C55" s="31" t="s">
+      <c r="C55" s="26"/>
+      <c r="D55" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="D55" s="32" t="s">
+      <c r="E55" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="E55" s="33" t="s">
+      <c r="F55" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="F55" s="34" t="s">
+      <c r="G55" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="G55" s="35" t="s">
+      <c r="H55" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="H55" s="36" t="s">
+      <c r="I55" s="32" t="s">
         <v>115</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="D1:I1"/>
     <mergeCell ref="A3:A22"/>
     <mergeCell ref="A23:A36"/>
     <mergeCell ref="A37:A55"/>
+    <mergeCell ref="C1:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Just to be sure the modifications are in.
</commit_message>
<xml_diff>
--- a/Notes/table_fetch_runner_locations.xlsx
+++ b/Notes/table_fetch_runner_locations.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="157">
   <si>
     <t>Type de course</t>
   </si>
@@ -615,7 +615,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -762,6 +762,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -2585,17 +2586,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C38" sqref="A38:XFD38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="41.140625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" style="14" customWidth="1"/>
-    <col min="6" max="6" width="36.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.5703125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="32" style="14" customWidth="1"/>
+    <col min="6" max="6" width="31" style="15" customWidth="1"/>
     <col min="7" max="7" width="36.42578125" style="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="36.42578125" style="17" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="36.42578125" style="18" bestFit="1" customWidth="1"/>
@@ -3461,28 +3462,28 @@
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="37"/>
-      <c r="B38" s="26" t="s">
+      <c r="B38" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="C38" s="26"/>
-      <c r="D38" s="27" t="s">
+      <c r="C38" s="45"/>
+      <c r="D38" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="E38" s="28" t="s">
+      <c r="E38" s="47" t="s">
         <v>150</v>
       </c>
-      <c r="F38" s="29" t="s">
+      <c r="F38" s="48" t="s">
         <v>150</v>
       </c>
-      <c r="G38" s="30" t="s">
+      <c r="G38" s="49" t="s">
         <v>150</v>
       </c>
-      <c r="H38" s="31" t="s">
+      <c r="H38" s="50" t="s">
         <v>150</v>
       </c>
-      <c r="I38" s="32" t="s">
+      <c r="I38" s="51" t="s">
         <v>150</v>
       </c>
     </row>
@@ -3491,7 +3492,9 @@
       <c r="B39" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="C39" s="26"/>
+      <c r="C39" s="26" t="s">
+        <v>156</v>
+      </c>
       <c r="D39" s="27" t="s">
         <v>151</v>
       </c>
@@ -3511,53 +3514,53 @@
         <v>151</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="37"/>
-      <c r="B40" s="26" t="s">
+      <c r="B40" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="C40" s="26"/>
-      <c r="D40" s="27" t="s">
+      <c r="C40" s="45"/>
+      <c r="D40" s="46" t="s">
         <v>152</v>
       </c>
-      <c r="E40" s="28" t="s">
+      <c r="E40" s="47" t="s">
         <v>152</v>
       </c>
-      <c r="F40" s="29" t="s">
+      <c r="F40" s="48" t="s">
         <v>152</v>
       </c>
-      <c r="G40" s="30" t="s">
+      <c r="G40" s="49" t="s">
         <v>152</v>
       </c>
-      <c r="H40" s="31" t="s">
+      <c r="H40" s="50" t="s">
         <v>152</v>
       </c>
-      <c r="I40" s="32" t="s">
+      <c r="I40" s="51" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="37"/>
-      <c r="B41" s="26" t="s">
+      <c r="B41" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="C41" s="26"/>
-      <c r="D41" s="27" t="s">
+      <c r="C41" s="45"/>
+      <c r="D41" s="46" t="s">
         <v>153</v>
       </c>
-      <c r="E41" s="28" t="s">
+      <c r="E41" s="47" t="s">
         <v>153</v>
       </c>
-      <c r="F41" s="29" t="s">
+      <c r="F41" s="48" t="s">
         <v>153</v>
       </c>
-      <c r="G41" s="30" t="s">
+      <c r="G41" s="49" t="s">
         <v>153</v>
       </c>
-      <c r="H41" s="31" t="s">
+      <c r="H41" s="50" t="s">
         <v>153</v>
       </c>
-      <c r="I41" s="32" t="s">
+      <c r="I41" s="51" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3566,7 +3569,9 @@
       <c r="B42" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="C42" s="26"/>
+      <c r="C42" s="26" t="s">
+        <v>156</v>
+      </c>
       <c r="D42" s="27" t="s">
         <v>154</v>
       </c>
@@ -3591,7 +3596,9 @@
       <c r="B43" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="C43" s="26"/>
+      <c r="C43" s="26" t="s">
+        <v>156</v>
+      </c>
       <c r="D43" s="27" t="s">
         <v>106</v>
       </c>
@@ -3616,7 +3623,9 @@
       <c r="B44" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="C44" s="26"/>
+      <c r="C44" s="53" t="s">
+        <v>156</v>
+      </c>
       <c r="D44" s="27" t="s">
         <v>107</v>
       </c>
@@ -3641,7 +3650,9 @@
       <c r="B45" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="C45" s="26"/>
+      <c r="C45" s="53" t="s">
+        <v>156</v>
+      </c>
       <c r="D45" s="27" t="s">
         <v>108</v>
       </c>
@@ -3666,7 +3677,9 @@
       <c r="B46" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="C46" s="26"/>
+      <c r="C46" s="53" t="s">
+        <v>156</v>
+      </c>
       <c r="D46" s="27" t="s">
         <v>109</v>
       </c>
@@ -3691,7 +3704,9 @@
       <c r="B47" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C47" s="26"/>
+      <c r="C47" s="53" t="s">
+        <v>156</v>
+      </c>
       <c r="D47" s="27" t="s">
         <v>110</v>
       </c>
@@ -3716,7 +3731,9 @@
       <c r="B48" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C48" s="26"/>
+      <c r="C48" s="53" t="s">
+        <v>156</v>
+      </c>
       <c r="D48" s="27" t="s">
         <v>111</v>
       </c>
@@ -3741,7 +3758,9 @@
       <c r="B49" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C49" s="26"/>
+      <c r="C49" s="53" t="s">
+        <v>156</v>
+      </c>
       <c r="D49" s="27" t="s">
         <v>112</v>
       </c>
@@ -3761,28 +3780,28 @@
         <v>112</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="37"/>
-      <c r="B50" s="26" t="s">
+      <c r="B50" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="C50" s="26"/>
-      <c r="D50" s="27" t="s">
+      <c r="C50" s="54"/>
+      <c r="D50" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="E50" s="28" t="s">
+      <c r="E50" s="47" t="s">
         <v>116</v>
       </c>
-      <c r="F50" s="29" t="s">
+      <c r="F50" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="G50" s="30" t="s">
+      <c r="G50" s="49" t="s">
         <v>116</v>
       </c>
-      <c r="H50" s="31" t="s">
+      <c r="H50" s="50" t="s">
         <v>116</v>
       </c>
-      <c r="I50" s="32" t="s">
+      <c r="I50" s="51" t="s">
         <v>116</v>
       </c>
     </row>
@@ -3791,7 +3810,9 @@
       <c r="B51" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="C51" s="26"/>
+      <c r="C51" s="53" t="s">
+        <v>156</v>
+      </c>
       <c r="D51" s="27" t="s">
         <v>117</v>
       </c>
@@ -3816,7 +3837,9 @@
       <c r="B52" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="C52" s="26"/>
+      <c r="C52" s="53" t="s">
+        <v>156</v>
+      </c>
       <c r="D52" s="27" t="s">
         <v>118</v>
       </c>
@@ -3841,7 +3864,9 @@
       <c r="B53" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="C53" s="26"/>
+      <c r="C53" s="53" t="s">
+        <v>156</v>
+      </c>
       <c r="D53" s="27" t="s">
         <v>113</v>
       </c>
@@ -3866,7 +3891,9 @@
       <c r="B54" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="C54" s="26"/>
+      <c r="C54" s="53" t="s">
+        <v>156</v>
+      </c>
       <c r="D54" s="27" t="s">
         <v>114</v>
       </c>
@@ -3891,7 +3918,9 @@
       <c r="B55" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="C55" s="26"/>
+      <c r="C55" s="53" t="s">
+        <v>156</v>
+      </c>
       <c r="D55" s="27" t="s">
         <v>115</v>
       </c>

</xml_diff>

<commit_message>
More notes and the start of the refactoring of fetch_runners.
</commit_message>
<xml_diff>
--- a/Notes/table_fetch_runner_locations.xlsx
+++ b/Notes/table_fetch_runner_locations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21855" windowHeight="11325" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21855" windowHeight="11325"/>
   </bookViews>
   <sheets>
     <sheet name="Partants" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="178">
   <si>
     <t>Type de course</t>
   </si>
@@ -130,9 +130,6 @@
     <t>Poids H. - Poids M.</t>
   </si>
   <si>
-    <t>Rapports prob.  first - last</t>
-  </si>
-  <si>
     <t>td[4]</t>
   </si>
   <si>
@@ -224,9 +221,6 @@
     <t>Red. Km</t>
   </si>
   <si>
-    <t>Rapports prob First - Last</t>
-  </si>
-  <si>
     <t>Commentaires d'après-course</t>
   </si>
   <si>
@@ -446,9 +440,6 @@
     <t>Distance</t>
   </si>
   <si>
-    <t>Rapports prob. First</t>
-  </si>
-  <si>
     <t>Rapports prob. Last</t>
   </si>
   <si>
@@ -504,6 +495,78 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>English name</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>shoes</t>
+  </si>
+  <si>
+    <t>blinder</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>jockey</t>
+  </si>
+  <si>
+    <t>trainer</t>
+  </si>
+  <si>
+    <t>earnings</t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t>load_handicap</t>
+  </si>
+  <si>
+    <t>load_ride</t>
+  </si>
+  <si>
+    <t>handicap</t>
+  </si>
+  <si>
+    <t>is_non_runner</t>
+  </si>
+  <si>
+    <t>is_favorite</t>
+  </si>
+  <si>
+    <t>is_replaced</t>
+  </si>
+  <si>
+    <t>pregnant</t>
+  </si>
+  <si>
+    <t>places</t>
+  </si>
+  <si>
+    <t>final_place</t>
+  </si>
+  <si>
+    <t>km_time</t>
+  </si>
+  <si>
+    <t>Rapports prob. Référence</t>
+  </si>
+  <si>
+    <t>Rapports prob Référence - Direct</t>
+  </si>
+  <si>
+    <t>Rapports prob. référence - direct</t>
   </si>
 </sst>
 </file>
@@ -708,18 +771,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -763,6 +814,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1046,8 +1109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1055,7 +1118,7 @@
     <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="29.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="50.140625" style="4" customWidth="1"/>
     <col min="6" max="6" width="42.5703125" customWidth="1"/>
   </cols>
@@ -1151,7 +1214,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D9" s="4" t="s">
-        <v>33</v>
+        <v>177</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>21</v>
@@ -1162,7 +1225,7 @@
         <v>22</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1175,10 +1238,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1189,7 +1252,7 @@
         <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>5</v>
@@ -1248,7 +1311,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D20" s="4" t="s">
-        <v>33</v>
+        <v>177</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>21</v>
@@ -1269,10 +1332,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D23" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1280,10 +1343,10 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" t="s">
         <v>37</v>
-      </c>
-      <c r="C24" t="s">
-        <v>38</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>5</v>
@@ -1297,12 +1360,12 @@
         <v>30</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D26" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>15</v>
@@ -1313,7 +1376,7 @@
         <v>7</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>18</v>
@@ -1324,7 +1387,7 @@
         <v>31</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1335,7 +1398,7 @@
         <v>26</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1348,7 +1411,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D31" s="4" t="s">
-        <v>33</v>
+        <v>177</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>21</v>
@@ -1369,21 +1432,21 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D34" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" t="s">
         <v>40</v>
-      </c>
-      <c r="B35" t="s">
-        <v>37</v>
-      </c>
-      <c r="C35" t="s">
-        <v>41</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>5</v>
@@ -1397,7 +1460,7 @@
         <v>30</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1413,7 +1476,7 @@
         <v>31</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1421,21 +1484,21 @@
         <v>32</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D40" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1446,12 +1509,12 @@
         <v>20</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D42" s="4" t="s">
-        <v>33</v>
+        <v>177</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>21</v>
@@ -1472,21 +1535,21 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D45" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E45" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>5</v>
@@ -1500,10 +1563,10 @@
         <v>30</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1522,7 +1585,7 @@
         <v>31</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1530,21 +1593,21 @@
         <v>32</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D51" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -1552,15 +1615,15 @@
         <v>11</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F52" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D53" s="4" t="s">
-        <v>33</v>
+        <v>177</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>21</v>
@@ -1581,21 +1644,21 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D56" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E56" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B57" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C57" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>5</v>
@@ -1609,7 +1672,7 @@
         <v>30</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -1625,7 +1688,7 @@
         <v>31</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -1633,12 +1696,12 @@
         <v>32</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D62" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E62" s="4" t="s">
         <v>26</v>
@@ -1649,12 +1712,12 @@
         <v>11</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D64" s="4" t="s">
-        <v>33</v>
+        <v>177</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>21</v>
@@ -1675,10 +1738,10 @@
     </row>
     <row r="67" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D67" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E67" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="E67" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1694,8 +1757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection sqref="A1:C68"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1731,16 +1794,16 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1761,39 +1824,39 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>63</v>
+        <v>176</v>
       </c>
       <c r="E7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1806,18 +1869,18 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1825,16 +1888,16 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1855,42 +1918,42 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>63</v>
+        <v>176</v>
       </c>
       <c r="E18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E20" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1903,18 +1966,18 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D23" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1922,16 +1985,16 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="D24" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1944,50 +2007,50 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
-        <v>63</v>
+        <v>176</v>
       </c>
       <c r="E29" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E31" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2000,35 +2063,35 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D34" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B35" t="s">
-        <v>37</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="D35" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -2041,50 +2104,50 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E38" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>63</v>
+        <v>176</v>
       </c>
       <c r="E40" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E41" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E42" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -2097,35 +2160,35 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D45" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -2138,50 +2201,50 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E49" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E50" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
-        <v>63</v>
+        <v>176</v>
       </c>
       <c r="E51" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E52" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E53" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -2194,35 +2257,35 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D56" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B57" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2235,50 +2298,50 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E59" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E60" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E61" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
-        <v>63</v>
+        <v>176</v>
       </c>
       <c r="E62" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E63" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E64" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2291,19 +2354,19 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E66" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C67" s="3"/>
       <c r="D67" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -2311,16 +2374,16 @@
         <v>29</v>
       </c>
       <c r="B68" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C68" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E68" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2352,213 +2415,213 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" t="s">
         <v>101</v>
-      </c>
-      <c r="C5" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B16" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B17" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B20" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" t="s">
         <v>40</v>
-      </c>
-      <c r="B36" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B58" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C58" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -2566,10 +2629,10 @@
         <v>29</v>
       </c>
       <c r="B69" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C69" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2584,1369 +2647,1466 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="29.5703125" style="13" customWidth="1"/>
-    <col min="5" max="5" width="32" style="14" customWidth="1"/>
-    <col min="6" max="6" width="31" style="15" customWidth="1"/>
-    <col min="7" max="7" width="36.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="29.5703125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="32" style="14" customWidth="1"/>
+    <col min="7" max="7" width="31" style="15" customWidth="1"/>
+    <col min="8" max="8" width="36.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.42578125" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="34" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="34" t="s">
-        <v>155</v>
-      </c>
-      <c r="D1" s="35" t="s">
+      <c r="C1" s="51" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" s="51" t="s">
+        <v>152</v>
+      </c>
+      <c r="E1" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="7" t="s">
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="I2" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
-        <v>119</v>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="51" t="s">
+        <v>117</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>156</v>
-      </c>
-      <c r="D3" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="F3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="G3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="H3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="I3" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="J3" s="18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="51"/>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C4" t="s">
         <v>156</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" t="s">
+        <v>153</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="51"/>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" t="s">
+        <v>153</v>
+      </c>
+      <c r="E5" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="F5" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="F4" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
-      <c r="B5" t="s">
+      <c r="G5" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="51"/>
+      <c r="B6" t="s">
         <v>122</v>
       </c>
-      <c r="C5" t="s">
-        <v>156</v>
-      </c>
-      <c r="D5" s="13" t="s">
+      <c r="C6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G6" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="H6" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="F5" s="15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
-      <c r="B6" t="s">
+      <c r="I6" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="51"/>
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" t="s">
+        <v>159</v>
+      </c>
+      <c r="D7" t="s">
+        <v>153</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="C6" t="s">
-        <v>156</v>
-      </c>
-      <c r="F6" s="15" t="s">
+      <c r="F7" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="G7" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="G6" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="I6" s="18" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" t="s">
-        <v>156</v>
-      </c>
-      <c r="D7" s="13" t="s">
+      <c r="H7" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="J7" s="18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="51"/>
+      <c r="B8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D8" t="s">
+        <v>153</v>
+      </c>
+      <c r="E8" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="F8" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="G8" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="H8" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="I8" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="J8" s="18" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
-      <c r="B8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" t="s">
-        <v>156</v>
-      </c>
-      <c r="D8" s="13" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="51"/>
+      <c r="B9" t="s">
         <v>128</v>
       </c>
-      <c r="E8" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="F8" s="15" t="s">
+      <c r="C9" t="s">
+        <v>161</v>
+      </c>
+      <c r="D9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E9" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="G8" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="H8" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
-      <c r="B9" t="s">
+      <c r="F9" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="C9" t="s">
-        <v>156</v>
-      </c>
-      <c r="D9" s="13" t="s">
+      <c r="G9" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="J9" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="51"/>
+      <c r="B10" t="s">
         <v>131</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="C10" t="s">
+        <v>162</v>
+      </c>
+      <c r="D10" t="s">
+        <v>153</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="F9" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="I9" s="18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
-      <c r="B10" t="s">
+      <c r="F10" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="J10" s="18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="51"/>
+      <c r="B11" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="C10" t="s">
-        <v>156</v>
-      </c>
-      <c r="D10" s="13" t="s">
+      <c r="C11" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="37"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="40"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="51"/>
+      <c r="B12" t="s">
         <v>134</v>
       </c>
-      <c r="E10" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="H10" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="I10" s="18" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
-      <c r="B11" s="38" t="s">
-        <v>135</v>
-      </c>
-      <c r="D11" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="41"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="44"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
-      <c r="B12" t="s">
-        <v>136</v>
-      </c>
       <c r="C12" t="s">
-        <v>156</v>
-      </c>
-      <c r="D12" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="D12" t="s">
+        <v>153</v>
+      </c>
+      <c r="E12" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="F12" s="14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="51"/>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>156</v>
-      </c>
-      <c r="D13" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="D13" t="s">
+        <v>153</v>
+      </c>
+      <c r="E13" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="F13" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="G13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="H13" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="I13" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="18" t="s">
+      <c r="J13" s="18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
-      <c r="B14" s="38" t="s">
+    <row r="14" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="51"/>
+      <c r="B14" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="E14" s="35"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="40"/>
+    </row>
+    <row r="15" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="51"/>
+      <c r="B15" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="E15" s="35"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="40"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="51"/>
+      <c r="B16" t="s">
+        <v>136</v>
+      </c>
+      <c r="C16" t="s">
+        <v>165</v>
+      </c>
+      <c r="D16" t="s">
+        <v>153</v>
+      </c>
+      <c r="G16" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="44"/>
-    </row>
-    <row r="15" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
-      <c r="B15" s="38" t="s">
+      <c r="H16" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="D15" s="39"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="43"/>
-      <c r="I15" s="44"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
-      <c r="B16" t="s">
+      <c r="I16" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="J16" s="18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="51"/>
+      <c r="B17" t="s">
         <v>139</v>
       </c>
-      <c r="C16" t="s">
-        <v>156</v>
-      </c>
-      <c r="F16" s="15" t="s">
+      <c r="C17" t="s">
+        <v>166</v>
+      </c>
+      <c r="D17" t="s">
+        <v>153</v>
+      </c>
+      <c r="G17" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="G16" s="16" t="s">
+      <c r="H17" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="H16" s="17" t="s">
+      <c r="I17" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="I16" s="18" t="s">
+      <c r="J17" s="18" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="34"/>
-      <c r="B17" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="51"/>
+      <c r="B18" t="s">
         <v>142</v>
       </c>
-      <c r="C17" t="s">
-        <v>156</v>
-      </c>
-      <c r="F17" s="15" t="s">
+      <c r="C18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D18" t="s">
+        <v>153</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" s="18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="51"/>
+      <c r="B19" t="s">
         <v>143</v>
       </c>
-      <c r="G17" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="H17" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="I17" s="18" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="34"/>
-      <c r="B18" t="s">
-        <v>145</v>
-      </c>
-      <c r="C18" t="s">
-        <v>156</v>
-      </c>
-      <c r="G18" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="H18" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="I18" s="18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="34"/>
-      <c r="B19" t="s">
-        <v>146</v>
-      </c>
       <c r="C19" t="s">
-        <v>156</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="G19" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="H19" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="I19" s="18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="34"/>
+        <v>168</v>
+      </c>
+      <c r="D19" t="s">
+        <v>153</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="I19" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J19" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="51"/>
       <c r="B20" t="s">
         <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>156</v>
-      </c>
-      <c r="D20" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="D20" t="s">
+        <v>153</v>
+      </c>
+      <c r="E20" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="F20" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="G20" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="H20" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H20" s="17" t="s">
+      <c r="I20" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="I20" s="18" t="s">
+      <c r="J20" s="18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="34"/>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="51"/>
       <c r="B21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" t="s">
+        <v>170</v>
+      </c>
+      <c r="D21" t="s">
+        <v>153</v>
+      </c>
+      <c r="E21" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C21" t="s">
-        <v>156</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="H21" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="I21" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
+      <c r="F21" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="J21" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="51"/>
       <c r="B22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" t="s">
+        <v>171</v>
+      </c>
+      <c r="D22" t="s">
+        <v>153</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="H22" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I22" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="J22" s="18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="53" t="s">
+        <v>144</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="F23" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="G23" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="H23" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="I23" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="J23" s="25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="54"/>
+      <c r="B24" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="I24" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="J24" s="47" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="54"/>
+      <c r="B25" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="C25" s="41"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="F25" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="G25" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="H25" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="I25" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="J25" s="47" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="54"/>
+      <c r="B26" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" s="41"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="F26" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="G26" s="44"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="47"/>
+    </row>
+    <row r="27" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="54"/>
+      <c r="B27" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="H27" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="I27" s="46" t="s">
+        <v>123</v>
+      </c>
+      <c r="J27" s="47" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="54"/>
+      <c r="B28" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="C28" s="41"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="F28" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="G28" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="H28" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="I28" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="J28" s="47" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="54"/>
+      <c r="B29" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E29" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="F29" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="G29" s="29"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="32"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="54"/>
+      <c r="B30" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E30" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="F30" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G30" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="H30" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="I30" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="J30" s="32" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="54"/>
+      <c r="B31" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E31" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="F31" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="G31" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="H31" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="I31" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="J31" s="32" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="54"/>
+      <c r="B32" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="26"/>
+      <c r="D32" s="49" t="s">
+        <v>153</v>
+      </c>
+      <c r="E32" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="G32" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="H32" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="I32" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="J32" s="32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="54"/>
+      <c r="B33" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" s="41"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="F33" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="G33" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="H33" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="I33" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="J33" s="47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="54"/>
+      <c r="B34" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="F34" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="G34" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="H34" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="I34" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="J34" s="47" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="54"/>
+      <c r="B35" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="41"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="F35" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="G35" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="H35" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="I35" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="J35" s="47" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="54"/>
+      <c r="B36" s="48" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="48"/>
+      <c r="D36" s="48"/>
+      <c r="E36" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="F36" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="G36" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="H36" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="I36" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="J36" s="47" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="B37" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="C22" t="s">
-        <v>156</v>
-      </c>
-      <c r="D22" s="13" t="s">
+      <c r="C37" s="33"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="F37" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="G37" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="G22" s="16" t="s">
+      <c r="H37" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="H22" s="17" t="s">
+      <c r="I37" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="I22" s="18" t="s">
+      <c r="J37" s="32" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="36" t="s">
+    <row r="38" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="54"/>
+      <c r="B38" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" s="41"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="42" t="s">
         <v>147</v>
       </c>
-      <c r="B23" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="D23" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="F23" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="G23" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="H23" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="I23" s="25" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="37"/>
-      <c r="B24" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="45"/>
-      <c r="D24" s="46" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24" s="49" t="s">
-        <v>12</v>
-      </c>
-      <c r="H24" s="50" t="s">
-        <v>12</v>
-      </c>
-      <c r="I24" s="51" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="37"/>
-      <c r="B25" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="C25" s="45"/>
-      <c r="D25" s="46" t="s">
-        <v>121</v>
-      </c>
-      <c r="E25" s="47" t="s">
-        <v>121</v>
-      </c>
-      <c r="F25" s="48" t="s">
-        <v>121</v>
-      </c>
-      <c r="G25" s="49" t="s">
-        <v>121</v>
-      </c>
-      <c r="H25" s="50" t="s">
-        <v>121</v>
-      </c>
-      <c r="I25" s="51" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="37"/>
-      <c r="B26" s="45" t="s">
-        <v>122</v>
-      </c>
-      <c r="C26" s="45"/>
-      <c r="D26" s="46" t="s">
-        <v>123</v>
-      </c>
-      <c r="E26" s="47" t="s">
-        <v>123</v>
-      </c>
-      <c r="F26" s="48"/>
-      <c r="G26" s="49"/>
-      <c r="H26" s="50"/>
-      <c r="I26" s="51"/>
-    </row>
-    <row r="27" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="37"/>
-      <c r="B27" s="45" t="s">
-        <v>124</v>
-      </c>
-      <c r="C27" s="45"/>
-      <c r="D27" s="46"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="48" t="s">
-        <v>125</v>
-      </c>
-      <c r="G27" s="49" t="s">
-        <v>125</v>
-      </c>
-      <c r="H27" s="50" t="s">
-        <v>125</v>
-      </c>
-      <c r="I27" s="51" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="37"/>
-      <c r="B28" s="45" t="s">
-        <v>130</v>
-      </c>
-      <c r="C28" s="45"/>
-      <c r="D28" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="E28" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="F28" s="48" t="s">
-        <v>72</v>
-      </c>
-      <c r="G28" s="49" t="s">
-        <v>72</v>
-      </c>
-      <c r="H28" s="50" t="s">
-        <v>72</v>
-      </c>
-      <c r="I28" s="51" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="37"/>
-      <c r="B29" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="D29" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="E29" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="F29" s="29"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="32"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="37"/>
-      <c r="B30" s="26" t="s">
-        <v>137</v>
-      </c>
-      <c r="C30" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="D30" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="E30" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="F30" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="G30" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="H30" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="I30" s="32" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="37"/>
-      <c r="B31" s="26" t="s">
-        <v>138</v>
-      </c>
-      <c r="C31" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="D31" s="27" t="s">
+      <c r="F38" s="43" t="s">
+        <v>147</v>
+      </c>
+      <c r="G38" s="44" t="s">
+        <v>147</v>
+      </c>
+      <c r="H38" s="45" t="s">
+        <v>147</v>
+      </c>
+      <c r="I38" s="46" t="s">
+        <v>147</v>
+      </c>
+      <c r="J38" s="47" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="54"/>
+      <c r="B39" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E39" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="F39" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="F31" s="29" t="s">
+      <c r="G39" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="G31" s="30" t="s">
+      <c r="H39" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="H31" s="31" t="s">
+      <c r="I39" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="I31" s="32" t="s">
+      <c r="J39" s="32" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="37"/>
-      <c r="B32" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="C32" s="53" t="s">
-        <v>156</v>
-      </c>
-      <c r="D32" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="E32" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="F32" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="G32" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="H32" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="I32" s="32" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="37"/>
-      <c r="B33" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="C33" s="45"/>
-      <c r="D33" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="E33" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="F33" s="48" t="s">
-        <v>70</v>
-      </c>
-      <c r="G33" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="H33" s="50" t="s">
-        <v>70</v>
-      </c>
-      <c r="I33" s="51" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="37"/>
-      <c r="B34" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="C34" s="45"/>
-      <c r="D34" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="E34" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="F34" s="48" t="s">
-        <v>28</v>
-      </c>
-      <c r="G34" s="49" t="s">
-        <v>28</v>
-      </c>
-      <c r="H34" s="50" t="s">
-        <v>28</v>
-      </c>
-      <c r="I34" s="51" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="37"/>
-      <c r="B35" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="C35" s="45"/>
-      <c r="D35" s="46" t="s">
-        <v>57</v>
-      </c>
-      <c r="E35" s="47" t="s">
-        <v>57</v>
-      </c>
-      <c r="F35" s="48" t="s">
-        <v>57</v>
-      </c>
-      <c r="G35" s="49" t="s">
-        <v>57</v>
-      </c>
-      <c r="H35" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="I35" s="51" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="37"/>
-      <c r="B36" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="C36" s="52"/>
-      <c r="D36" s="46" t="s">
-        <v>77</v>
-      </c>
-      <c r="E36" s="47" t="s">
-        <v>77</v>
-      </c>
-      <c r="F36" s="48" t="s">
-        <v>77</v>
-      </c>
-      <c r="G36" s="49" t="s">
-        <v>77</v>
-      </c>
-      <c r="H36" s="50" t="s">
-        <v>77</v>
-      </c>
-      <c r="I36" s="51" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="36" t="s">
+    <row r="40" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="54"/>
+      <c r="B40" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40" s="41"/>
+      <c r="D40" s="41"/>
+      <c r="E40" s="42" t="s">
         <v>149</v>
       </c>
-      <c r="B37" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="C37" s="33"/>
-      <c r="D37" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="E37" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="F37" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="G37" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="H37" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="I37" s="32" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="37"/>
-      <c r="B38" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="C38" s="45"/>
-      <c r="D38" s="46" t="s">
+      <c r="F40" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="G40" s="44" t="s">
+        <v>149</v>
+      </c>
+      <c r="H40" s="45" t="s">
+        <v>149</v>
+      </c>
+      <c r="I40" s="46" t="s">
+        <v>149</v>
+      </c>
+      <c r="J40" s="47" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="54"/>
+      <c r="B41" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" s="41"/>
+      <c r="D41" s="41"/>
+      <c r="E41" s="42" t="s">
         <v>150</v>
       </c>
-      <c r="E38" s="47" t="s">
+      <c r="F41" s="43" t="s">
         <v>150</v>
       </c>
-      <c r="F38" s="48" t="s">
+      <c r="G41" s="44" t="s">
         <v>150</v>
       </c>
-      <c r="G38" s="49" t="s">
+      <c r="H41" s="45" t="s">
         <v>150</v>
       </c>
-      <c r="H38" s="50" t="s">
+      <c r="I41" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="I38" s="51" t="s">
+      <c r="J41" s="47" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="37"/>
-      <c r="B39" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="C39" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="D39" s="27" t="s">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="54"/>
+      <c r="B42" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E42" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="E39" s="28" t="s">
+      <c r="F42" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="F39" s="29" t="s">
+      <c r="G42" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="G39" s="30" t="s">
+      <c r="H42" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="H39" s="31" t="s">
+      <c r="I42" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="I39" s="32" t="s">
+      <c r="J42" s="32" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="37"/>
-      <c r="B40" s="45" t="s">
-        <v>82</v>
-      </c>
-      <c r="C40" s="45"/>
-      <c r="D40" s="46" t="s">
-        <v>152</v>
-      </c>
-      <c r="E40" s="47" t="s">
-        <v>152</v>
-      </c>
-      <c r="F40" s="48" t="s">
-        <v>152</v>
-      </c>
-      <c r="G40" s="49" t="s">
-        <v>152</v>
-      </c>
-      <c r="H40" s="50" t="s">
-        <v>152</v>
-      </c>
-      <c r="I40" s="51" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="37"/>
-      <c r="B41" s="45" t="s">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="54"/>
+      <c r="B43" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="C41" s="45"/>
-      <c r="D41" s="46" t="s">
+      <c r="C43" s="26"/>
+      <c r="D43" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="E41" s="47" t="s">
+      <c r="E43" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="F43" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="G43" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="H43" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="I43" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="J43" s="32" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="54"/>
+      <c r="B44" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" s="26"/>
+      <c r="D44" s="49" t="s">
         <v>153</v>
       </c>
-      <c r="F41" s="48" t="s">
+      <c r="E44" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="F44" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="G44" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="H44" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="I44" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="J44" s="32" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="54"/>
+      <c r="B45" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C45" s="26"/>
+      <c r="D45" s="49" t="s">
         <v>153</v>
       </c>
-      <c r="G41" s="49" t="s">
+      <c r="E45" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="F45" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="G45" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="H45" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="I45" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="J45" s="32" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="54"/>
+      <c r="B46" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C46" s="26"/>
+      <c r="D46" s="49" t="s">
         <v>153</v>
       </c>
-      <c r="H41" s="50" t="s">
+      <c r="E46" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="F46" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="G46" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="H46" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="I46" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="J46" s="32" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="54"/>
+      <c r="B47" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="C47" s="26"/>
+      <c r="D47" s="49" t="s">
         <v>153</v>
       </c>
-      <c r="I41" s="51" t="s">
+      <c r="E47" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="F47" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="G47" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="H47" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="I47" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="J47" s="32" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="54"/>
+      <c r="B48" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C48" s="26"/>
+      <c r="D48" s="49" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="37"/>
-      <c r="B42" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="C42" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="D42" s="27" t="s">
-        <v>154</v>
-      </c>
-      <c r="E42" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="F42" s="29" t="s">
-        <v>154</v>
-      </c>
-      <c r="G42" s="30" t="s">
-        <v>154</v>
-      </c>
-      <c r="H42" s="31" t="s">
-        <v>154</v>
-      </c>
-      <c r="I42" s="32" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="37"/>
-      <c r="B43" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="C43" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="D43" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="E43" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="F43" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="G43" s="30" t="s">
-        <v>106</v>
-      </c>
-      <c r="H43" s="31" t="s">
-        <v>106</v>
-      </c>
-      <c r="I43" s="32" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="37"/>
-      <c r="B44" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="C44" s="53" t="s">
-        <v>156</v>
-      </c>
-      <c r="D44" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="E44" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="F44" s="29" t="s">
-        <v>107</v>
-      </c>
-      <c r="G44" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="H44" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="I44" s="32" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="37"/>
-      <c r="B45" s="26" t="s">
+      <c r="E48" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="F48" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="G48" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="H48" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="I48" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="J48" s="32" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="54"/>
+      <c r="B49" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="C45" s="53" t="s">
-        <v>156</v>
-      </c>
-      <c r="D45" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="E45" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="F45" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="G45" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="H45" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="I45" s="32" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="37"/>
-      <c r="B46" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="C46" s="53" t="s">
-        <v>156</v>
-      </c>
-      <c r="D46" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="E46" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="F46" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="G46" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="H46" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="I46" s="32" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="37"/>
-      <c r="B47" s="26" t="s">
+      <c r="C49" s="26"/>
+      <c r="D49" s="49" t="s">
+        <v>153</v>
+      </c>
+      <c r="E49" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="F49" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="G49" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="H49" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="I49" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="J49" s="32" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="54"/>
+      <c r="B50" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="C47" s="53" t="s">
-        <v>156</v>
-      </c>
-      <c r="D47" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="E47" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="F47" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="G47" s="30" t="s">
-        <v>110</v>
-      </c>
-      <c r="H47" s="31" t="s">
-        <v>110</v>
-      </c>
-      <c r="I47" s="32" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="37"/>
-      <c r="B48" s="26" t="s">
+      <c r="C50" s="41"/>
+      <c r="D50" s="50"/>
+      <c r="E50" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="F50" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="G50" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="H50" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="I50" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="J50" s="47" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="54"/>
+      <c r="B51" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C48" s="53" t="s">
-        <v>156</v>
-      </c>
-      <c r="D48" s="27" t="s">
+      <c r="C51" s="26"/>
+      <c r="D51" s="49" t="s">
+        <v>153</v>
+      </c>
+      <c r="E51" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="F51" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="G51" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="H51" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="I51" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="J51" s="32" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="54"/>
+      <c r="B52" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="C52" s="26"/>
+      <c r="D52" s="49" t="s">
+        <v>153</v>
+      </c>
+      <c r="E52" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="F52" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="G52" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="H52" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="I52" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="J52" s="32" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="54"/>
+      <c r="B53" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C53" s="26"/>
+      <c r="D53" s="49" t="s">
+        <v>153</v>
+      </c>
+      <c r="E53" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="E48" s="28" t="s">
+      <c r="F53" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="F48" s="29" t="s">
+      <c r="G53" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="G48" s="30" t="s">
+      <c r="H53" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="H48" s="31" t="s">
+      <c r="I53" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="I48" s="32" t="s">
+      <c r="J53" s="32" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="37"/>
-      <c r="B49" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="C49" s="53" t="s">
-        <v>156</v>
-      </c>
-      <c r="D49" s="27" t="s">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="54"/>
+      <c r="B54" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="C54" s="26"/>
+      <c r="D54" s="49" t="s">
+        <v>153</v>
+      </c>
+      <c r="E54" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="E49" s="28" t="s">
+      <c r="F54" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="F49" s="29" t="s">
+      <c r="G54" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="G49" s="30" t="s">
+      <c r="H54" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="H49" s="31" t="s">
+      <c r="I54" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="I49" s="32" t="s">
+      <c r="J54" s="32" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="50" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="37"/>
-      <c r="B50" s="45" t="s">
-        <v>91</v>
-      </c>
-      <c r="C50" s="54"/>
-      <c r="D50" s="46" t="s">
-        <v>116</v>
-      </c>
-      <c r="E50" s="47" t="s">
-        <v>116</v>
-      </c>
-      <c r="F50" s="48" t="s">
-        <v>116</v>
-      </c>
-      <c r="G50" s="49" t="s">
-        <v>116</v>
-      </c>
-      <c r="H50" s="50" t="s">
-        <v>116</v>
-      </c>
-      <c r="I50" s="51" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="37"/>
-      <c r="B51" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="C51" s="53" t="s">
-        <v>156</v>
-      </c>
-      <c r="D51" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="E51" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="F51" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="G51" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="H51" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="I51" s="32" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="37"/>
-      <c r="B52" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="C52" s="53" t="s">
-        <v>156</v>
-      </c>
-      <c r="D52" s="27" t="s">
-        <v>118</v>
-      </c>
-      <c r="E52" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="F52" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="G52" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="H52" s="31" t="s">
-        <v>118</v>
-      </c>
-      <c r="I52" s="32" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="37"/>
-      <c r="B53" s="26" t="s">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="54"/>
+      <c r="B55" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="C53" s="53" t="s">
-        <v>156</v>
-      </c>
-      <c r="D53" s="27" t="s">
+      <c r="C55" s="26"/>
+      <c r="D55" s="49" t="s">
+        <v>153</v>
+      </c>
+      <c r="E55" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="E53" s="28" t="s">
+      <c r="F55" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="F53" s="29" t="s">
+      <c r="G55" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="G53" s="30" t="s">
+      <c r="H55" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="H53" s="31" t="s">
+      <c r="I55" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="I53" s="32" t="s">
+      <c r="J55" s="32" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="37"/>
-      <c r="B54" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="C54" s="53" t="s">
-        <v>156</v>
-      </c>
-      <c r="D54" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="E54" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="F54" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="G54" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="H54" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="I54" s="32" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="37"/>
-      <c r="B55" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="C55" s="53" t="s">
-        <v>156</v>
-      </c>
-      <c r="D55" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="E55" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="F55" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="G55" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="H55" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="I55" s="32" t="s">
-        <v>115</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="E1:J1"/>
     <mergeCell ref="A3:A22"/>
     <mergeCell ref="A23:A36"/>
     <mergeCell ref="A37:A55"/>
+    <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Forgot to save before commit.
</commit_message>
<xml_diff>
--- a/Notes/table_fetch_runner_locations.xlsx
+++ b/Notes/table_fetch_runner_locations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21855" windowHeight="11325"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21855" windowHeight="11325" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Partants" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="195">
   <si>
     <t>Type de course</t>
   </si>
@@ -440,9 +440,6 @@
     <t>Distance</t>
   </si>
   <si>
-    <t>Rapports prob. Last</t>
-  </si>
-  <si>
     <t>Poids H.</t>
   </si>
   <si>
@@ -524,12 +521,12 @@
     <t>trainer</t>
   </si>
   <si>
-    <t>earnings</t>
-  </si>
-  <si>
     <t>distance</t>
   </si>
   <si>
+    <t>history</t>
+  </si>
+  <si>
     <t>load_handicap</t>
   </si>
   <si>
@@ -567,6 +564,60 @@
   </si>
   <si>
     <t>Rapports prob. référence - direct</t>
+  </si>
+  <si>
+    <t>Rapports prob. Direct</t>
+  </si>
+  <si>
+    <t>odds_ref</t>
+  </si>
+  <si>
+    <t>odds_direct</t>
+  </si>
+  <si>
+    <t>commentary</t>
+  </si>
+  <si>
+    <t>race</t>
+  </si>
+  <si>
+    <t>coat</t>
+  </si>
+  <si>
+    <t>races_run</t>
+  </si>
+  <si>
+    <t>victories</t>
+  </si>
+  <si>
+    <t>earnings_career</t>
+  </si>
+  <si>
+    <t>Gains N</t>
+  </si>
+  <si>
+    <t>earnings_current_year</t>
+  </si>
+  <si>
+    <t>earnings_last_year</t>
+  </si>
+  <si>
+    <t>earnings_victory</t>
+  </si>
+  <si>
+    <t>owner</t>
+  </si>
+  <si>
+    <t>breeder</t>
+  </si>
+  <si>
+    <t>father</t>
+  </si>
+  <si>
+    <t>mother</t>
+  </si>
+  <si>
+    <t>mother's father</t>
   </si>
 </sst>
 </file>
@@ -1109,7 +1160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -1214,7 +1265,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D9" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>21</v>
@@ -1311,7 +1362,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D20" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>21</v>
@@ -1411,7 +1462,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D31" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>21</v>
@@ -1514,7 +1565,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D42" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>21</v>
@@ -1623,7 +1674,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D53" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>21</v>
@@ -1717,7 +1768,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D64" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>21</v>
@@ -1840,7 +1891,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E7" t="s">
         <v>65</v>
@@ -1934,7 +1985,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E18" t="s">
         <v>65</v>
@@ -2031,7 +2082,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E29" t="s">
         <v>65</v>
@@ -2128,7 +2179,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E40" t="s">
         <v>65</v>
@@ -2225,7 +2276,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E51" t="s">
         <v>65</v>
@@ -2322,7 +2373,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E62" t="s">
         <v>65</v>
@@ -2649,8 +2700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C3:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2671,10 +2722,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="51" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E1" s="52" t="s">
         <v>3</v>
@@ -2716,10 +2767,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>12</v>
@@ -2746,10 +2797,10 @@
         <v>118</v>
       </c>
       <c r="C4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>119</v>
@@ -2776,10 +2827,10 @@
         <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>121</v>
@@ -2797,10 +2848,10 @@
         <v>122</v>
       </c>
       <c r="C6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G6" s="15" t="s">
         <v>123</v>
@@ -2821,10 +2872,10 @@
         <v>80</v>
       </c>
       <c r="C7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>124</v>
@@ -2851,10 +2902,10 @@
         <v>81</v>
       </c>
       <c r="C8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>126</v>
@@ -2881,10 +2932,10 @@
         <v>128</v>
       </c>
       <c r="C9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>129</v>
@@ -2911,10 +2962,10 @@
         <v>131</v>
       </c>
       <c r="C10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>132</v>
@@ -2940,9 +2991,6 @@
       <c r="B11" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="C11" s="34" t="s">
-        <v>163</v>
-      </c>
       <c r="E11" s="35" t="s">
         <v>19</v>
       </c>
@@ -2960,10 +3008,10 @@
         <v>134</v>
       </c>
       <c r="C12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>26</v>
@@ -2978,10 +3026,10 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>20</v>
@@ -3005,7 +3053,7 @@
     <row r="14" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="51"/>
       <c r="B14" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E14" s="35"/>
       <c r="F14" s="36"/>
@@ -3017,7 +3065,7 @@
     <row r="15" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="51"/>
       <c r="B15" s="34" t="s">
-        <v>135</v>
+        <v>177</v>
       </c>
       <c r="E15" s="35"/>
       <c r="F15" s="36"/>
@@ -3029,61 +3077,61 @@
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="51"/>
       <c r="B16" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" t="s">
+        <v>164</v>
+      </c>
+      <c r="D16" t="s">
+        <v>152</v>
+      </c>
+      <c r="G16" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="C16" t="s">
-        <v>165</v>
-      </c>
-      <c r="D16" t="s">
-        <v>153</v>
-      </c>
-      <c r="G16" s="15" t="s">
+      <c r="H16" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H16" s="16" t="s">
-        <v>138</v>
-      </c>
       <c r="I16" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J16" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="51"/>
       <c r="B17" t="s">
+        <v>138</v>
+      </c>
+      <c r="C17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D17" t="s">
+        <v>152</v>
+      </c>
+      <c r="G17" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="C17" t="s">
-        <v>166</v>
-      </c>
-      <c r="D17" t="s">
-        <v>153</v>
-      </c>
-      <c r="G17" s="15" t="s">
+      <c r="H17" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="H17" s="16" t="s">
-        <v>141</v>
-      </c>
       <c r="I17" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J17" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="51"/>
       <c r="B18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H18" s="16" t="s">
         <v>26</v>
@@ -3098,13 +3146,13 @@
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="51"/>
       <c r="B19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E19" s="13" t="s">
         <v>45</v>
@@ -3131,10 +3179,10 @@
         <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>28</v>
@@ -3161,10 +3209,10 @@
         <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E21" s="13" t="s">
         <v>56</v>
@@ -3191,10 +3239,10 @@
         <v>74</v>
       </c>
       <c r="C22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E22" s="13" t="s">
         <v>75</v>
@@ -3217,16 +3265,16 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="53" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B23" s="19" t="s">
         <v>58</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E23" s="20" t="s">
         <v>63</v>
@@ -3371,10 +3419,10 @@
         <v>61</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E29" s="27" t="s">
         <v>42</v>
@@ -3390,11 +3438,13 @@
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="54"/>
       <c r="B30" s="26" t="s">
-        <v>175</v>
-      </c>
-      <c r="C30" s="26"/>
+        <v>174</v>
+      </c>
+      <c r="C30" s="26" t="s">
+        <v>178</v>
+      </c>
       <c r="D30" s="26" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E30" s="27" t="s">
         <v>44</v>
@@ -3418,29 +3468,31 @@
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="54"/>
       <c r="B31" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="C31" s="26"/>
+        <v>177</v>
+      </c>
+      <c r="C31" s="26" t="s">
+        <v>179</v>
+      </c>
       <c r="D31" s="26" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E31" s="27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F31" s="28" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G31" s="29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H31" s="30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I31" s="31" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J31" s="32" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -3448,9 +3500,11 @@
       <c r="B32" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="26"/>
+      <c r="C32" s="26" t="s">
+        <v>180</v>
+      </c>
       <c r="D32" s="49" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E32" s="27" t="s">
         <v>66</v>
@@ -3577,7 +3631,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="53" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B37" s="33" t="s">
         <v>76</v>
@@ -3611,22 +3665,22 @@
       <c r="C38" s="41"/>
       <c r="D38" s="41"/>
       <c r="E38" s="42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F38" s="43" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G38" s="44" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H38" s="45" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I38" s="46" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J38" s="47" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -3634,27 +3688,29 @@
       <c r="B39" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="C39" s="26"/>
+      <c r="C39" s="26" t="s">
+        <v>181</v>
+      </c>
       <c r="D39" s="26" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E39" s="27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F39" s="28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G39" s="29" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H39" s="30" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I39" s="31" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J39" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
@@ -3665,22 +3721,22 @@
       <c r="C40" s="41"/>
       <c r="D40" s="41"/>
       <c r="E40" s="42" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F40" s="43" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G40" s="44" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H40" s="45" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I40" s="46" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J40" s="47" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="41" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
@@ -3691,22 +3747,22 @@
       <c r="C41" s="41"/>
       <c r="D41" s="41"/>
       <c r="E41" s="42" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F41" s="43" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G41" s="44" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H41" s="45" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I41" s="46" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J41" s="47" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -3714,27 +3770,29 @@
       <c r="B42" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="C42" s="26"/>
+      <c r="C42" s="26" t="s">
+        <v>182</v>
+      </c>
       <c r="D42" s="26" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E42" s="27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F42" s="28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G42" s="29" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H42" s="30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I42" s="31" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J42" s="32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -3742,9 +3800,11 @@
       <c r="B43" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="C43" s="26"/>
+      <c r="C43" s="26" t="s">
+        <v>183</v>
+      </c>
       <c r="D43" s="26" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E43" s="27" t="s">
         <v>104</v>
@@ -3770,9 +3830,11 @@
       <c r="B44" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="C44" s="26"/>
+      <c r="C44" s="26" t="s">
+        <v>184</v>
+      </c>
       <c r="D44" s="49" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E44" s="27" t="s">
         <v>105</v>
@@ -3798,9 +3860,11 @@
       <c r="B45" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="C45" s="26"/>
+      <c r="C45" s="26" t="s">
+        <v>171</v>
+      </c>
       <c r="D45" s="49" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E45" s="27" t="s">
         <v>106</v>
@@ -3826,9 +3890,11 @@
       <c r="B46" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="C46" s="26"/>
+      <c r="C46" s="26" t="s">
+        <v>185</v>
+      </c>
       <c r="D46" s="49" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E46" s="27" t="s">
         <v>107</v>
@@ -3854,9 +3920,11 @@
       <c r="B47" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="C47" s="26"/>
+      <c r="C47" s="26" t="s">
+        <v>188</v>
+      </c>
       <c r="D47" s="49" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E47" s="27" t="s">
         <v>108</v>
@@ -3882,9 +3950,11 @@
       <c r="B48" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="C48" s="26"/>
+      <c r="C48" s="26" t="s">
+        <v>189</v>
+      </c>
       <c r="D48" s="49" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E48" s="27" t="s">
         <v>109</v>
@@ -3908,11 +3978,13 @@
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="54"/>
       <c r="B49" s="26" t="s">
-        <v>87</v>
-      </c>
-      <c r="C49" s="26"/>
+        <v>186</v>
+      </c>
+      <c r="C49" s="26" t="s">
+        <v>187</v>
+      </c>
       <c r="D49" s="49" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E49" s="27" t="s">
         <v>110</v>
@@ -3964,9 +4036,11 @@
       <c r="B51" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C51" s="26"/>
+      <c r="C51" s="26" t="s">
+        <v>190</v>
+      </c>
       <c r="D51" s="49" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E51" s="27" t="s">
         <v>115</v>
@@ -3992,9 +4066,11 @@
       <c r="B52" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="C52" s="26"/>
+      <c r="C52" s="26" t="s">
+        <v>191</v>
+      </c>
       <c r="D52" s="49" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E52" s="27" t="s">
         <v>116</v>
@@ -4020,9 +4096,11 @@
       <c r="B53" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="C53" s="26"/>
+      <c r="C53" s="26" t="s">
+        <v>192</v>
+      </c>
       <c r="D53" s="49" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E53" s="27" t="s">
         <v>111</v>
@@ -4048,9 +4126,11 @@
       <c r="B54" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="C54" s="26"/>
+      <c r="C54" s="26" t="s">
+        <v>193</v>
+      </c>
       <c r="D54" s="49" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E54" s="27" t="s">
         <v>112</v>
@@ -4076,9 +4156,11 @@
       <c r="B55" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="C55" s="26"/>
+      <c r="C55" s="26" t="s">
+        <v>194</v>
+      </c>
       <c r="D55" s="49" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E55" s="27" t="s">
         <v>113</v>

</xml_diff>

<commit_message>
Adds column map data and brings get_column_map up to date.
</commit_message>
<xml_diff>
--- a/Notes/table_fetch_runner_locations.xlsx
+++ b/Notes/table_fetch_runner_locations.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="196">
   <si>
     <t>Type de course</t>
   </si>
@@ -422,12 +422,6 @@
     <t>Jokey (Driver)</t>
   </si>
   <si>
-    <t>pan.participants-driver</t>
-  </si>
-  <si>
-    <t>pan.participants-jokey</t>
-  </si>
-  <si>
     <t>Entraineur</t>
   </si>
   <si>
@@ -618,6 +612,15 @@
   </si>
   <si>
     <t>mother's father</t>
+  </si>
+  <si>
+    <t>Col Map</t>
+  </si>
+  <si>
+    <t>T/F</t>
+  </si>
+  <si>
+    <t>Loc</t>
   </si>
 </sst>
 </file>
@@ -657,7 +660,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -706,6 +709,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -729,7 +738,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -877,6 +886,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1265,7 +1276,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D9" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>21</v>
@@ -1362,7 +1373,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D20" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>21</v>
@@ -1462,7 +1473,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D31" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>21</v>
@@ -1565,7 +1576,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D42" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>21</v>
@@ -1674,7 +1685,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D53" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>21</v>
@@ -1768,7 +1779,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D64" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>21</v>
@@ -1891,7 +1902,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E7" t="s">
         <v>65</v>
@@ -1985,7 +1996,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E18" t="s">
         <v>65</v>
@@ -2082,7 +2093,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E29" t="s">
         <v>65</v>
@@ -2179,7 +2190,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E40" t="s">
         <v>65</v>
@@ -2276,7 +2287,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E51" t="s">
         <v>65</v>
@@ -2373,7 +2384,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E62" t="s">
         <v>65</v>
@@ -2698,68 +2709,73 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C3:C22"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="29.5703125" style="13" customWidth="1"/>
-    <col min="6" max="6" width="32" style="14" customWidth="1"/>
-    <col min="7" max="7" width="31" style="15" customWidth="1"/>
-    <col min="8" max="8" width="36.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.5703125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="32" style="14" customWidth="1"/>
+    <col min="8" max="8" width="31" style="15" customWidth="1"/>
+    <col min="9" max="9" width="36.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.42578125" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" s="51" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="51" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>151</v>
-      </c>
-      <c r="E1" s="52" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="51" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="52"/>
       <c r="G1" s="52"/>
       <c r="H1" s="52"/>
       <c r="I1" s="52"/>
       <c r="J1" s="52"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="52"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" s="51"/>
       <c r="C2" s="51"/>
       <c r="D2" s="51"/>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="51"/>
+      <c r="F2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="I2" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="J2" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="K2" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
         <v>117</v>
       </c>
@@ -2767,1429 +2783,1490 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D3" t="s">
-        <v>152</v>
-      </c>
-      <c r="E3" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="G3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="H3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="I3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="J3" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="K3" s="18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="51"/>
       <c r="B4" t="s">
         <v>118</v>
       </c>
       <c r="C4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D4" t="s">
-        <v>152</v>
-      </c>
-      <c r="E4" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="F4" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="G4" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="H4" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="I4" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="J4" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="K4" s="18" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="51"/>
       <c r="B5" t="s">
         <v>120</v>
       </c>
-      <c r="C5" t="s">
-        <v>156</v>
+      <c r="C5" s="55" t="s">
+        <v>154</v>
       </c>
       <c r="D5" t="s">
-        <v>152</v>
-      </c>
-      <c r="E5" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="E5" t="s">
+        <v>194</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="G5" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="H5" s="15" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="51"/>
       <c r="B6" t="s">
         <v>122</v>
       </c>
-      <c r="C6" t="s">
-        <v>157</v>
+      <c r="C6" s="55" t="s">
+        <v>155</v>
       </c>
       <c r="D6" t="s">
-        <v>152</v>
-      </c>
-      <c r="G6" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="E6" t="s">
+        <v>194</v>
+      </c>
+      <c r="H6" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="I6" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="J6" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="K6" s="18" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="51"/>
       <c r="B7" t="s">
         <v>80</v>
       </c>
-      <c r="C7" t="s">
-        <v>158</v>
+      <c r="C7" s="55" t="s">
+        <v>156</v>
       </c>
       <c r="D7" t="s">
-        <v>152</v>
-      </c>
-      <c r="E7" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="E7" t="s">
+        <v>195</v>
+      </c>
+      <c r="F7" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="G7" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="H7" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="I7" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="J7" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="J7" s="18" t="s">
+      <c r="K7" s="18" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="51"/>
       <c r="B8" t="s">
         <v>81</v>
       </c>
-      <c r="C8" t="s">
-        <v>159</v>
+      <c r="C8" s="55" t="s">
+        <v>157</v>
       </c>
       <c r="D8" t="s">
-        <v>152</v>
-      </c>
-      <c r="E8" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="E8" t="s">
+        <v>195</v>
+      </c>
+      <c r="F8" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="G8" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="H8" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="I8" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="J8" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="J8" s="18" t="s">
+      <c r="K8" s="18" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="51"/>
       <c r="B9" t="s">
         <v>128</v>
       </c>
-      <c r="C9" t="s">
-        <v>160</v>
+      <c r="C9" s="55" t="s">
+        <v>158</v>
       </c>
       <c r="D9" t="s">
-        <v>152</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="G9" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="E9" t="s">
+        <v>195</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="I9" s="17" t="s">
+      <c r="I9" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="J9" s="18" t="s">
+      <c r="J9" s="17" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="51"/>
       <c r="B10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D10" t="s">
-        <v>152</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="I10" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="J10" s="18" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="51"/>
       <c r="B11" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="E11" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="F11" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="36" t="s">
+      <c r="G11" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="37"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="40"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H11" s="37"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="40"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="51"/>
       <c r="B12" t="s">
-        <v>134</v>
-      </c>
-      <c r="C12" t="s">
-        <v>162</v>
+        <v>132</v>
+      </c>
+      <c r="C12" s="55" t="s">
+        <v>160</v>
       </c>
       <c r="D12" t="s">
-        <v>152</v>
-      </c>
-      <c r="E12" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="E12" t="s">
+        <v>194</v>
+      </c>
+      <c r="F12" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="G12" s="14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="51"/>
       <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C13" t="s">
-        <v>163</v>
+      <c r="C13" s="56" t="s">
+        <v>161</v>
       </c>
       <c r="D13" t="s">
-        <v>152</v>
-      </c>
-      <c r="E13" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="F13" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="G13" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="H13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="I13" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="17" t="s">
+      <c r="J13" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="18" t="s">
+      <c r="K13" s="18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="51"/>
       <c r="B14" s="34" t="s">
-        <v>174</v>
-      </c>
-      <c r="E14" s="35"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="40"/>
-    </row>
-    <row r="15" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+      <c r="F14" s="35"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="40"/>
+    </row>
+    <row r="15" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="51"/>
       <c r="B15" s="34" t="s">
-        <v>177</v>
-      </c>
-      <c r="E15" s="35"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="40"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+      <c r="F15" s="35"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="40"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="51"/>
       <c r="B16" t="s">
+        <v>133</v>
+      </c>
+      <c r="C16" s="55" t="s">
+        <v>162</v>
+      </c>
+      <c r="D16" t="s">
+        <v>150</v>
+      </c>
+      <c r="E16" t="s">
+        <v>195</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="I16" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="C16" t="s">
-        <v>164</v>
-      </c>
-      <c r="D16" t="s">
-        <v>152</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="I16" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="J16" s="18" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J16" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="K16" s="18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="51"/>
       <c r="B17" t="s">
+        <v>136</v>
+      </c>
+      <c r="C17" s="55" t="s">
+        <v>163</v>
+      </c>
+      <c r="D17" t="s">
+        <v>150</v>
+      </c>
+      <c r="E17" t="s">
+        <v>195</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="I17" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="C17" t="s">
-        <v>165</v>
-      </c>
-      <c r="D17" t="s">
-        <v>152</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="H17" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="I17" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="J17" s="18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J17" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="K17" s="18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="51"/>
       <c r="B18" t="s">
-        <v>141</v>
-      </c>
-      <c r="C18" t="s">
-        <v>166</v>
+        <v>139</v>
+      </c>
+      <c r="C18" s="55" t="s">
+        <v>164</v>
       </c>
       <c r="D18" t="s">
-        <v>152</v>
-      </c>
-      <c r="H18" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="E18" t="s">
+        <v>194</v>
+      </c>
+      <c r="I18" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="I18" s="17" t="s">
+      <c r="J18" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="J18" s="18" t="s">
+      <c r="K18" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="51"/>
       <c r="B19" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C19" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D19" t="s">
-        <v>152</v>
-      </c>
-      <c r="E19" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="F19" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="G19" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="G19" s="15" t="s">
+      <c r="H19" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="H19" s="16" t="s">
+      <c r="I19" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="17" t="s">
+      <c r="J19" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="J19" s="18" t="s">
+      <c r="K19" s="18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="51"/>
       <c r="B20" t="s">
         <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D20" t="s">
-        <v>152</v>
-      </c>
-      <c r="E20" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="F20" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="G20" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="H20" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="H20" s="16" t="s">
+      <c r="I20" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="I20" s="17" t="s">
+      <c r="J20" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="J20" s="18" t="s">
+      <c r="K20" s="18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="51"/>
       <c r="B21" t="s">
         <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D21" t="s">
-        <v>152</v>
-      </c>
-      <c r="E21" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="F21" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="G21" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="G21" s="15" t="s">
+      <c r="H21" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="H21" s="16" t="s">
+      <c r="I21" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="I21" s="17" t="s">
+      <c r="J21" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="J21" s="18" t="s">
+      <c r="K21" s="18" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="51"/>
       <c r="B22" t="s">
         <v>74</v>
       </c>
       <c r="C22" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D22" t="s">
-        <v>152</v>
-      </c>
-      <c r="E22" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="F22" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="F22" s="14" t="s">
+      <c r="G22" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="G22" s="15" t="s">
+      <c r="H22" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="H22" s="16" t="s">
+      <c r="I22" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="I22" s="17" t="s">
+      <c r="J22" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="J22" s="18" t="s">
+      <c r="K22" s="18" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="53" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B23" s="19" t="s">
         <v>58</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="E23" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="E23" s="19"/>
+      <c r="F23" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="F23" s="21" t="s">
+      <c r="G23" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="G23" s="22" t="s">
+      <c r="H23" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="H23" s="23" t="s">
+      <c r="I23" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="I23" s="24" t="s">
+      <c r="J23" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="J23" s="25" t="s">
+      <c r="K23" s="25" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="54"/>
       <c r="B24" s="41" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="41"/>
       <c r="D24" s="41"/>
-      <c r="E24" s="42" t="s">
+      <c r="E24" s="41"/>
+      <c r="F24" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="43" t="s">
+      <c r="G24" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="G24" s="44" t="s">
+      <c r="H24" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="H24" s="45" t="s">
+      <c r="I24" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="I24" s="46" t="s">
+      <c r="J24" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="J24" s="47" t="s">
+      <c r="K24" s="47" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="54"/>
       <c r="B25" s="41" t="s">
         <v>118</v>
       </c>
       <c r="C25" s="41"/>
       <c r="D25" s="41"/>
-      <c r="E25" s="42" t="s">
+      <c r="E25" s="41"/>
+      <c r="F25" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="F25" s="43" t="s">
+      <c r="G25" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="G25" s="44" t="s">
+      <c r="H25" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="H25" s="45" t="s">
+      <c r="I25" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="I25" s="46" t="s">
+      <c r="J25" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="J25" s="47" t="s">
+      <c r="K25" s="47" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="54"/>
       <c r="B26" s="41" t="s">
         <v>120</v>
       </c>
       <c r="C26" s="41"/>
       <c r="D26" s="41"/>
-      <c r="E26" s="42" t="s">
+      <c r="E26" s="41"/>
+      <c r="F26" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="F26" s="43" t="s">
+      <c r="G26" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="G26" s="44"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="46"/>
-      <c r="J26" s="47"/>
-    </row>
-    <row r="27" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H26" s="44"/>
+      <c r="I26" s="45"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="47"/>
+    </row>
+    <row r="27" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="54"/>
       <c r="B27" s="41" t="s">
         <v>122</v>
       </c>
       <c r="C27" s="41"/>
       <c r="D27" s="41"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="44" t="s">
+      <c r="E27" s="41"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="H27" s="45" t="s">
+      <c r="I27" s="45" t="s">
         <v>123</v>
       </c>
-      <c r="I27" s="46" t="s">
+      <c r="J27" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="J27" s="47" t="s">
+      <c r="K27" s="47" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="54"/>
       <c r="B28" s="41" t="s">
         <v>128</v>
       </c>
       <c r="C28" s="41"/>
       <c r="D28" s="41"/>
-      <c r="E28" s="42" t="s">
+      <c r="E28" s="41"/>
+      <c r="F28" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="F28" s="43" t="s">
+      <c r="G28" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="G28" s="44" t="s">
+      <c r="H28" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="H28" s="45" t="s">
+      <c r="I28" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="I28" s="46" t="s">
+      <c r="J28" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="J28" s="47" t="s">
+      <c r="K28" s="47" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="54"/>
       <c r="B29" s="26" t="s">
         <v>61</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="E29" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="E29" s="26"/>
+      <c r="F29" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="F29" s="28" t="s">
+      <c r="G29" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="G29" s="29"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="32"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H29" s="29"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="32"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="54"/>
       <c r="B30" s="26" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="E30" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="E30" s="26"/>
+      <c r="F30" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F30" s="28" t="s">
+      <c r="G30" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="G30" s="29" t="s">
+      <c r="H30" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="H30" s="30" t="s">
+      <c r="I30" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="I30" s="31" t="s">
+      <c r="J30" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J30" s="32" t="s">
+      <c r="K30" s="32" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="54"/>
       <c r="B31" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="C31" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="C31" s="26" t="s">
-        <v>179</v>
-      </c>
       <c r="D31" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="E31" s="27" t="s">
-        <v>144</v>
-      </c>
-      <c r="F31" s="28" t="s">
-        <v>144</v>
-      </c>
-      <c r="G31" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="H31" s="30" t="s">
-        <v>144</v>
-      </c>
-      <c r="I31" s="31" t="s">
-        <v>144</v>
-      </c>
-      <c r="J31" s="32" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="E31" s="26"/>
+      <c r="F31" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="G31" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="H31" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="I31" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="J31" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="K31" s="32" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="54"/>
       <c r="B32" s="26" t="s">
         <v>62</v>
       </c>
       <c r="C32" s="26" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D32" s="49" t="s">
-        <v>152</v>
-      </c>
-      <c r="E32" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="E32" s="49"/>
+      <c r="F32" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="F32" s="28" t="s">
+      <c r="G32" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="G32" s="29" t="s">
+      <c r="H32" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="H32" s="30" t="s">
+      <c r="I32" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="I32" s="31" t="s">
+      <c r="J32" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="J32" s="32" t="s">
+      <c r="K32" s="32" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="54"/>
       <c r="B33" s="41" t="s">
         <v>67</v>
       </c>
       <c r="C33" s="41"/>
       <c r="D33" s="41"/>
-      <c r="E33" s="42" t="s">
+      <c r="E33" s="41"/>
+      <c r="F33" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="F33" s="43" t="s">
+      <c r="G33" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="G33" s="44" t="s">
+      <c r="H33" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="H33" s="45" t="s">
+      <c r="I33" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="I33" s="46" t="s">
+      <c r="J33" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="J33" s="47" t="s">
+      <c r="K33" s="47" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="54"/>
       <c r="B34" s="41" t="s">
         <v>27</v>
       </c>
       <c r="C34" s="41"/>
       <c r="D34" s="41"/>
-      <c r="E34" s="42" t="s">
+      <c r="E34" s="41"/>
+      <c r="F34" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="F34" s="43" t="s">
+      <c r="G34" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="G34" s="44" t="s">
+      <c r="H34" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="H34" s="45" t="s">
+      <c r="I34" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="I34" s="46" t="s">
+      <c r="J34" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="J34" s="47" t="s">
+      <c r="K34" s="47" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="54"/>
       <c r="B35" s="41" t="s">
         <v>72</v>
       </c>
       <c r="C35" s="41"/>
       <c r="D35" s="41"/>
-      <c r="E35" s="42" t="s">
+      <c r="E35" s="41"/>
+      <c r="F35" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="F35" s="43" t="s">
+      <c r="G35" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="G35" s="44" t="s">
+      <c r="H35" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="H35" s="45" t="s">
+      <c r="I35" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="I35" s="46" t="s">
+      <c r="J35" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="J35" s="47" t="s">
+      <c r="K35" s="47" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="54"/>
       <c r="B36" s="48" t="s">
         <v>74</v>
       </c>
       <c r="C36" s="48"/>
       <c r="D36" s="48"/>
-      <c r="E36" s="42" t="s">
+      <c r="E36" s="48"/>
+      <c r="F36" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="F36" s="43" t="s">
+      <c r="G36" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="G36" s="44" t="s">
+      <c r="H36" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="H36" s="45" t="s">
+      <c r="I36" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="I36" s="46" t="s">
+      <c r="J36" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="J36" s="47" t="s">
+      <c r="K36" s="47" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="53" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B37" s="33" t="s">
         <v>76</v>
       </c>
       <c r="C37" s="33"/>
       <c r="D37" s="33"/>
-      <c r="E37" s="20" t="s">
+      <c r="E37" s="33"/>
+      <c r="F37" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="F37" s="21" t="s">
+      <c r="G37" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="G37" s="22" t="s">
+      <c r="H37" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="H37" s="23" t="s">
+      <c r="I37" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="I37" s="24" t="s">
+      <c r="J37" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="J37" s="32" t="s">
+      <c r="K37" s="32" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="54"/>
       <c r="B38" s="41" t="s">
         <v>118</v>
       </c>
       <c r="C38" s="41"/>
       <c r="D38" s="41"/>
-      <c r="E38" s="42" t="s">
-        <v>146</v>
-      </c>
-      <c r="F38" s="43" t="s">
-        <v>146</v>
-      </c>
-      <c r="G38" s="44" t="s">
-        <v>146</v>
-      </c>
-      <c r="H38" s="45" t="s">
-        <v>146</v>
-      </c>
-      <c r="I38" s="46" t="s">
-        <v>146</v>
-      </c>
-      <c r="J38" s="47" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E38" s="41"/>
+      <c r="F38" s="42" t="s">
+        <v>144</v>
+      </c>
+      <c r="G38" s="43" t="s">
+        <v>144</v>
+      </c>
+      <c r="H38" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="I38" s="45" t="s">
+        <v>144</v>
+      </c>
+      <c r="J38" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="K38" s="47" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="54"/>
       <c r="B39" s="26" t="s">
         <v>79</v>
       </c>
       <c r="C39" s="26" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D39" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="E39" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="F39" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="G39" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="H39" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="I39" s="31" t="s">
-        <v>147</v>
-      </c>
-      <c r="J39" s="32" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="E39" s="26"/>
+      <c r="F39" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="G39" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="H39" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="I39" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="J39" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="K39" s="32" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="54"/>
       <c r="B40" s="41" t="s">
         <v>80</v>
       </c>
       <c r="C40" s="41"/>
       <c r="D40" s="41"/>
-      <c r="E40" s="42" t="s">
-        <v>148</v>
-      </c>
-      <c r="F40" s="43" t="s">
-        <v>148</v>
-      </c>
-      <c r="G40" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="H40" s="45" t="s">
-        <v>148</v>
-      </c>
-      <c r="I40" s="46" t="s">
-        <v>148</v>
-      </c>
-      <c r="J40" s="47" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E40" s="41"/>
+      <c r="F40" s="42" t="s">
+        <v>146</v>
+      </c>
+      <c r="G40" s="43" t="s">
+        <v>146</v>
+      </c>
+      <c r="H40" s="44" t="s">
+        <v>146</v>
+      </c>
+      <c r="I40" s="45" t="s">
+        <v>146</v>
+      </c>
+      <c r="J40" s="46" t="s">
+        <v>146</v>
+      </c>
+      <c r="K40" s="47" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="54"/>
       <c r="B41" s="41" t="s">
         <v>81</v>
       </c>
       <c r="C41" s="41"/>
       <c r="D41" s="41"/>
-      <c r="E41" s="42" t="s">
-        <v>149</v>
-      </c>
-      <c r="F41" s="43" t="s">
-        <v>149</v>
-      </c>
-      <c r="G41" s="44" t="s">
-        <v>149</v>
-      </c>
-      <c r="H41" s="45" t="s">
-        <v>149</v>
-      </c>
-      <c r="I41" s="46" t="s">
-        <v>149</v>
-      </c>
-      <c r="J41" s="47" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E41" s="41"/>
+      <c r="F41" s="42" t="s">
+        <v>147</v>
+      </c>
+      <c r="G41" s="43" t="s">
+        <v>147</v>
+      </c>
+      <c r="H41" s="44" t="s">
+        <v>147</v>
+      </c>
+      <c r="I41" s="45" t="s">
+        <v>147</v>
+      </c>
+      <c r="J41" s="46" t="s">
+        <v>147</v>
+      </c>
+      <c r="K41" s="47" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="54"/>
       <c r="B42" s="26" t="s">
         <v>82</v>
       </c>
       <c r="C42" s="26" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D42" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="E42" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="F42" s="28" t="s">
-        <v>150</v>
-      </c>
-      <c r="G42" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="H42" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="I42" s="31" t="s">
-        <v>150</v>
-      </c>
-      <c r="J42" s="32" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E42" s="26"/>
+      <c r="F42" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="G42" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="H42" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="I42" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="J42" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="K42" s="32" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="54"/>
       <c r="B43" s="26" t="s">
         <v>83</v>
       </c>
       <c r="C43" s="26" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="E43" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="E43" s="26"/>
+      <c r="F43" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="F43" s="28" t="s">
+      <c r="G43" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="G43" s="29" t="s">
+      <c r="H43" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="H43" s="30" t="s">
+      <c r="I43" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="I43" s="31" t="s">
+      <c r="J43" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="J43" s="32" t="s">
+      <c r="K43" s="32" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="54"/>
       <c r="B44" s="26" t="s">
         <v>84</v>
       </c>
       <c r="C44" s="26" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D44" s="49" t="s">
-        <v>152</v>
-      </c>
-      <c r="E44" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="E44" s="49"/>
+      <c r="F44" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="F44" s="28" t="s">
+      <c r="G44" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="G44" s="29" t="s">
+      <c r="H44" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="H44" s="30" t="s">
+      <c r="I44" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="I44" s="31" t="s">
+      <c r="J44" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="J44" s="32" t="s">
+      <c r="K44" s="32" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="54"/>
       <c r="B45" s="26" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="26" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D45" s="49" t="s">
-        <v>152</v>
-      </c>
-      <c r="E45" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="E45" s="49"/>
+      <c r="F45" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="F45" s="28" t="s">
+      <c r="G45" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="G45" s="29" t="s">
+      <c r="H45" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="H45" s="30" t="s">
+      <c r="I45" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="I45" s="31" t="s">
+      <c r="J45" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="J45" s="32" t="s">
+      <c r="K45" s="32" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="54"/>
       <c r="B46" s="26" t="s">
         <v>86</v>
       </c>
       <c r="C46" s="26" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D46" s="49" t="s">
-        <v>152</v>
-      </c>
-      <c r="E46" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="E46" s="49"/>
+      <c r="F46" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="F46" s="28" t="s">
+      <c r="G46" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="G46" s="29" t="s">
+      <c r="H46" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="H46" s="30" t="s">
+      <c r="I46" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="I46" s="31" t="s">
+      <c r="J46" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="J46" s="32" t="s">
+      <c r="K46" s="32" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="54"/>
       <c r="B47" s="26" t="s">
         <v>87</v>
       </c>
       <c r="C47" s="26" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D47" s="49" t="s">
-        <v>152</v>
-      </c>
-      <c r="E47" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="E47" s="49"/>
+      <c r="F47" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="F47" s="28" t="s">
+      <c r="G47" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="G47" s="29" t="s">
+      <c r="H47" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="H47" s="30" t="s">
+      <c r="I47" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="I47" s="31" t="s">
+      <c r="J47" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="J47" s="32" t="s">
+      <c r="K47" s="32" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="54"/>
       <c r="B48" s="26" t="s">
         <v>88</v>
       </c>
       <c r="C48" s="26" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D48" s="49" t="s">
-        <v>152</v>
-      </c>
-      <c r="E48" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="E48" s="49"/>
+      <c r="F48" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="F48" s="28" t="s">
+      <c r="G48" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="G48" s="29" t="s">
+      <c r="H48" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="H48" s="30" t="s">
+      <c r="I48" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="I48" s="31" t="s">
+      <c r="J48" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="J48" s="32" t="s">
+      <c r="K48" s="32" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="54"/>
       <c r="B49" s="26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C49" s="26" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D49" s="49" t="s">
-        <v>152</v>
-      </c>
-      <c r="E49" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="E49" s="49"/>
+      <c r="F49" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F49" s="28" t="s">
+      <c r="G49" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="G49" s="29" t="s">
+      <c r="H49" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="H49" s="30" t="s">
+      <c r="I49" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="I49" s="31" t="s">
+      <c r="J49" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="J49" s="32" t="s">
+      <c r="K49" s="32" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="50" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="54"/>
       <c r="B50" s="41" t="s">
         <v>89</v>
       </c>
       <c r="C50" s="41"/>
       <c r="D50" s="50"/>
-      <c r="E50" s="42" t="s">
+      <c r="E50" s="50"/>
+      <c r="F50" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="F50" s="43" t="s">
+      <c r="G50" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="G50" s="44" t="s">
+      <c r="H50" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="H50" s="45" t="s">
+      <c r="I50" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="I50" s="46" t="s">
+      <c r="J50" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="J50" s="47" t="s">
+      <c r="K50" s="47" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="54"/>
       <c r="B51" s="26" t="s">
         <v>90</v>
       </c>
       <c r="C51" s="26" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D51" s="49" t="s">
-        <v>152</v>
-      </c>
-      <c r="E51" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="E51" s="49"/>
+      <c r="F51" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="F51" s="28" t="s">
+      <c r="G51" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="G51" s="29" t="s">
+      <c r="H51" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="H51" s="30" t="s">
+      <c r="I51" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="I51" s="31" t="s">
+      <c r="J51" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="J51" s="32" t="s">
+      <c r="K51" s="32" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="54"/>
       <c r="B52" s="26" t="s">
         <v>91</v>
       </c>
       <c r="C52" s="26" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D52" s="49" t="s">
-        <v>152</v>
-      </c>
-      <c r="E52" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="E52" s="49"/>
+      <c r="F52" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="F52" s="28" t="s">
+      <c r="G52" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="G52" s="29" t="s">
+      <c r="H52" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="H52" s="30" t="s">
+      <c r="I52" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="I52" s="31" t="s">
+      <c r="J52" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="J52" s="32" t="s">
+      <c r="K52" s="32" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="54"/>
       <c r="B53" s="26" t="s">
         <v>92</v>
       </c>
       <c r="C53" s="26" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D53" s="49" t="s">
-        <v>152</v>
-      </c>
-      <c r="E53" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="E53" s="49"/>
+      <c r="F53" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="F53" s="28" t="s">
+      <c r="G53" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="G53" s="29" t="s">
+      <c r="H53" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="H53" s="30" t="s">
+      <c r="I53" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="I53" s="31" t="s">
+      <c r="J53" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="J53" s="32" t="s">
+      <c r="K53" s="32" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="54"/>
       <c r="B54" s="26" t="s">
         <v>93</v>
       </c>
       <c r="C54" s="26" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D54" s="49" t="s">
-        <v>152</v>
-      </c>
-      <c r="E54" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="E54" s="49"/>
+      <c r="F54" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="F54" s="28" t="s">
+      <c r="G54" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="G54" s="29" t="s">
+      <c r="H54" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="H54" s="30" t="s">
+      <c r="I54" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="I54" s="31" t="s">
+      <c r="J54" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="J54" s="32" t="s">
+      <c r="K54" s="32" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="54"/>
       <c r="B55" s="26" t="s">
         <v>94</v>
       </c>
       <c r="C55" s="26" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D55" s="49" t="s">
-        <v>152</v>
-      </c>
-      <c r="E55" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="E55" s="49"/>
+      <c r="F55" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="F55" s="28" t="s">
+      <c r="G55" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="G55" s="29" t="s">
+      <c r="H55" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="H55" s="30" t="s">
+      <c r="I55" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="I55" s="31" t="s">
+      <c r="J55" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="J55" s="32" t="s">
+      <c r="K55" s="32" t="s">
         <v>113</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="F1:K1"/>
     <mergeCell ref="A3:A22"/>
     <mergeCell ref="A23:A36"/>
     <mergeCell ref="A37:A55"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finishes fetch_runner_shallow and starts fetch_resul_shallow. Also fixed the result table mapping.
</commit_message>
<xml_diff>
--- a/Notes/table_fetch_runner_locations.xlsx
+++ b/Notes/table_fetch_runner_locations.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="196">
   <si>
     <t>Type de course</t>
   </si>
@@ -738,7 +738,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -874,6 +874,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -886,8 +888,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1171,7 +1172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -2712,7 +2713,7 @@
   <dimension ref="A1:K55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2730,32 +2731,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="53" t="s">
         <v>151</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="53" t="s">
         <v>149</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="53" t="s">
         <v>193</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
       <c r="F2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2776,7 +2777,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="53" t="s">
         <v>117</v>
       </c>
       <c r="B3" t="s">
@@ -2808,7 +2809,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="51"/>
+      <c r="A4" s="53"/>
       <c r="B4" t="s">
         <v>118</v>
       </c>
@@ -2838,11 +2839,11 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="51"/>
+      <c r="A5" s="53"/>
       <c r="B5" t="s">
         <v>120</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="51" t="s">
         <v>154</v>
       </c>
       <c r="D5" t="s">
@@ -2862,11 +2863,11 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="51"/>
+      <c r="A6" s="53"/>
       <c r="B6" t="s">
         <v>122</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="51" t="s">
         <v>155</v>
       </c>
       <c r="D6" t="s">
@@ -2889,11 +2890,11 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="51"/>
+      <c r="A7" s="53"/>
       <c r="B7" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="51" t="s">
         <v>156</v>
       </c>
       <c r="D7" t="s">
@@ -2922,11 +2923,11 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="51"/>
+      <c r="A8" s="53"/>
       <c r="B8" t="s">
         <v>81</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="51" t="s">
         <v>157</v>
       </c>
       <c r="D8" t="s">
@@ -2955,11 +2956,11 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="51"/>
+      <c r="A9" s="53"/>
       <c r="B9" t="s">
         <v>128</v>
       </c>
-      <c r="C9" s="55" t="s">
+      <c r="C9" s="51" t="s">
         <v>158</v>
       </c>
       <c r="D9" t="s">
@@ -2988,7 +2989,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="51"/>
+      <c r="A10" s="53"/>
       <c r="B10" t="s">
         <v>129</v>
       </c>
@@ -3018,7 +3019,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="51"/>
+      <c r="A11" s="53"/>
       <c r="B11" s="34" t="s">
         <v>131</v>
       </c>
@@ -3034,11 +3035,11 @@
       <c r="K11" s="40"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="51"/>
+      <c r="A12" s="53"/>
       <c r="B12" t="s">
         <v>132</v>
       </c>
-      <c r="C12" s="55" t="s">
+      <c r="C12" s="51" t="s">
         <v>160</v>
       </c>
       <c r="D12" t="s">
@@ -3055,11 +3056,11 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="51"/>
+      <c r="A13" s="53"/>
       <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="56" t="s">
+      <c r="C13" s="52" t="s">
         <v>161</v>
       </c>
       <c r="D13" t="s">
@@ -3085,7 +3086,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="51"/>
+      <c r="A14" s="53"/>
       <c r="B14" s="34" t="s">
         <v>172</v>
       </c>
@@ -3097,7 +3098,7 @@
       <c r="K14" s="40"/>
     </row>
     <row r="15" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="51"/>
+      <c r="A15" s="53"/>
       <c r="B15" s="34" t="s">
         <v>175</v>
       </c>
@@ -3109,11 +3110,11 @@
       <c r="K15" s="40"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="51"/>
+      <c r="A16" s="53"/>
       <c r="B16" t="s">
         <v>133</v>
       </c>
-      <c r="C16" s="55" t="s">
+      <c r="C16" s="51" t="s">
         <v>162</v>
       </c>
       <c r="D16" t="s">
@@ -3136,11 +3137,11 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="51"/>
+      <c r="A17" s="53"/>
       <c r="B17" t="s">
         <v>136</v>
       </c>
-      <c r="C17" s="55" t="s">
+      <c r="C17" s="51" t="s">
         <v>163</v>
       </c>
       <c r="D17" t="s">
@@ -3163,11 +3164,11 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="51"/>
+      <c r="A18" s="53"/>
       <c r="B18" t="s">
         <v>139</v>
       </c>
-      <c r="C18" s="55" t="s">
+      <c r="C18" s="51" t="s">
         <v>164</v>
       </c>
       <c r="D18" t="s">
@@ -3187,7 +3188,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="51"/>
+      <c r="A19" s="53"/>
       <c r="B19" t="s">
         <v>140</v>
       </c>
@@ -3217,7 +3218,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="51"/>
+      <c r="A20" s="53"/>
       <c r="B20" t="s">
         <v>27</v>
       </c>
@@ -3247,7 +3248,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="51"/>
+      <c r="A21" s="53"/>
       <c r="B21" t="s">
         <v>55</v>
       </c>
@@ -3277,7 +3278,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="51"/>
+      <c r="A22" s="53"/>
       <c r="B22" t="s">
         <v>74</v>
       </c>
@@ -3307,7 +3308,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="53" t="s">
+      <c r="A23" s="55" t="s">
         <v>141</v>
       </c>
       <c r="B23" s="19" t="s">
@@ -3340,7 +3341,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="54"/>
+      <c r="A24" s="56"/>
       <c r="B24" s="41" t="s">
         <v>5</v>
       </c>
@@ -3367,7 +3368,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="54"/>
+      <c r="A25" s="56"/>
       <c r="B25" s="41" t="s">
         <v>118</v>
       </c>
@@ -3394,7 +3395,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="54"/>
+      <c r="A26" s="56"/>
       <c r="B26" s="41" t="s">
         <v>120</v>
       </c>
@@ -3413,7 +3414,7 @@
       <c r="K26" s="47"/>
     </row>
     <row r="27" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="54"/>
+      <c r="A27" s="56"/>
       <c r="B27" s="41" t="s">
         <v>122</v>
       </c>
@@ -3436,7 +3437,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="54"/>
+      <c r="A28" s="56"/>
       <c r="B28" s="41" t="s">
         <v>128</v>
       </c>
@@ -3463,17 +3464,19 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="54"/>
+      <c r="A29" s="56"/>
       <c r="B29" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="26" t="s">
+      <c r="C29" s="57" t="s">
         <v>171</v>
       </c>
       <c r="D29" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="E29" s="26"/>
+      <c r="E29" s="26" t="s">
+        <v>194</v>
+      </c>
       <c r="F29" s="27" t="s">
         <v>42</v>
       </c>
@@ -3486,7 +3489,7 @@
       <c r="K29" s="32"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="54"/>
+      <c r="A30" s="56"/>
       <c r="B30" s="26" t="s">
         <v>172</v>
       </c>
@@ -3517,7 +3520,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="54"/>
+      <c r="A31" s="56"/>
       <c r="B31" s="26" t="s">
         <v>175</v>
       </c>
@@ -3548,7 +3551,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="54"/>
+      <c r="A32" s="56"/>
       <c r="B32" s="26" t="s">
         <v>62</v>
       </c>
@@ -3579,7 +3582,7 @@
       </c>
     </row>
     <row r="33" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="54"/>
+      <c r="A33" s="56"/>
       <c r="B33" s="41" t="s">
         <v>67</v>
       </c>
@@ -3606,7 +3609,7 @@
       </c>
     </row>
     <row r="34" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="54"/>
+      <c r="A34" s="56"/>
       <c r="B34" s="41" t="s">
         <v>27</v>
       </c>
@@ -3633,7 +3636,7 @@
       </c>
     </row>
     <row r="35" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="54"/>
+      <c r="A35" s="56"/>
       <c r="B35" s="41" t="s">
         <v>72</v>
       </c>
@@ -3660,7 +3663,7 @@
       </c>
     </row>
     <row r="36" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="54"/>
+      <c r="A36" s="56"/>
       <c r="B36" s="48" t="s">
         <v>74</v>
       </c>
@@ -3687,7 +3690,7 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="53" t="s">
+      <c r="A37" s="55" t="s">
         <v>143</v>
       </c>
       <c r="B37" s="33" t="s">
@@ -3716,7 +3719,7 @@
       </c>
     </row>
     <row r="38" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="54"/>
+      <c r="A38" s="56"/>
       <c r="B38" s="41" t="s">
         <v>118</v>
       </c>
@@ -3743,7 +3746,7 @@
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="54"/>
+      <c r="A39" s="56"/>
       <c r="B39" s="26" t="s">
         <v>79</v>
       </c>
@@ -3774,7 +3777,7 @@
       </c>
     </row>
     <row r="40" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="54"/>
+      <c r="A40" s="56"/>
       <c r="B40" s="41" t="s">
         <v>80</v>
       </c>
@@ -3801,7 +3804,7 @@
       </c>
     </row>
     <row r="41" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="54"/>
+      <c r="A41" s="56"/>
       <c r="B41" s="41" t="s">
         <v>81</v>
       </c>
@@ -3828,7 +3831,7 @@
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="54"/>
+      <c r="A42" s="56"/>
       <c r="B42" s="26" t="s">
         <v>82</v>
       </c>
@@ -3859,7 +3862,7 @@
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="54"/>
+      <c r="A43" s="56"/>
       <c r="B43" s="26" t="s">
         <v>83</v>
       </c>
@@ -3890,7 +3893,7 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="54"/>
+      <c r="A44" s="56"/>
       <c r="B44" s="26" t="s">
         <v>84</v>
       </c>
@@ -3921,7 +3924,7 @@
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="54"/>
+      <c r="A45" s="56"/>
       <c r="B45" s="26" t="s">
         <v>85</v>
       </c>
@@ -3952,7 +3955,7 @@
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="54"/>
+      <c r="A46" s="56"/>
       <c r="B46" s="26" t="s">
         <v>86</v>
       </c>
@@ -3983,7 +3986,7 @@
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="54"/>
+      <c r="A47" s="56"/>
       <c r="B47" s="26" t="s">
         <v>87</v>
       </c>
@@ -4014,7 +4017,7 @@
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="54"/>
+      <c r="A48" s="56"/>
       <c r="B48" s="26" t="s">
         <v>88</v>
       </c>
@@ -4045,7 +4048,7 @@
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="54"/>
+      <c r="A49" s="56"/>
       <c r="B49" s="26" t="s">
         <v>184</v>
       </c>
@@ -4076,7 +4079,7 @@
       </c>
     </row>
     <row r="50" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="54"/>
+      <c r="A50" s="56"/>
       <c r="B50" s="41" t="s">
         <v>89</v>
       </c>
@@ -4103,7 +4106,7 @@
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="54"/>
+      <c r="A51" s="56"/>
       <c r="B51" s="26" t="s">
         <v>90</v>
       </c>
@@ -4134,7 +4137,7 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="54"/>
+      <c r="A52" s="56"/>
       <c r="B52" s="26" t="s">
         <v>91</v>
       </c>
@@ -4165,7 +4168,7 @@
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="54"/>
+      <c r="A53" s="56"/>
       <c r="B53" s="26" t="s">
         <v>92</v>
       </c>
@@ -4196,7 +4199,7 @@
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="54"/>
+      <c r="A54" s="56"/>
       <c r="B54" s="26" t="s">
         <v>93</v>
       </c>
@@ -4227,7 +4230,7 @@
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="54"/>
+      <c r="A55" s="56"/>
       <c r="B55" s="26" t="s">
         <v>94</v>
       </c>

</xml_diff>

<commit_message>
Corrects the get_column_map so it deals with slight variations. Also changes so that a horse's sex and age are to be fetched in fetch_runner_deep (rather than fetch_runner_shallow) so they're not missed for non-runners.
</commit_message>
<xml_diff>
--- a/Notes/table_fetch_runner_locations.xlsx
+++ b/Notes/table_fetch_runner_locations.xlsx
@@ -2712,8 +2712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adds fetch_runner_deep. Seems to be a problem sometimes when the race is finished, the runners table doesn't load fast enough and the reacetype is not recognized. Relatively rare hopefully.
</commit_message>
<xml_diff>
--- a/Notes/table_fetch_runner_locations.xlsx
+++ b/Notes/table_fetch_runner_locations.xlsx
@@ -627,7 +627,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -653,6 +653,13 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color theme="1" tint="0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1" tint="0.249977111117893"/>
       <name val="Calibri"/>
@@ -738,7 +745,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -876,6 +883,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -888,7 +898,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -2712,8 +2721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2722,7 +2731,7 @@
     <col min="3" max="3" width="14.85546875" customWidth="1"/>
     <col min="4" max="4" width="7.42578125" customWidth="1"/>
     <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.5703125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="55.28515625" style="13" customWidth="1"/>
     <col min="7" max="7" width="32" style="14" customWidth="1"/>
     <col min="8" max="8" width="31" style="15" customWidth="1"/>
     <col min="9" max="9" width="36.42578125" style="16" bestFit="1" customWidth="1"/>
@@ -2731,32 +2740,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="56" t="s">
         <v>151</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="56" t="s">
         <v>149</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="56" t="s">
         <v>193</v>
       </c>
-      <c r="F1" s="54" t="s">
+      <c r="F1" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
       <c r="F2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2777,7 +2786,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="56" t="s">
         <v>117</v>
       </c>
       <c r="B3" t="s">
@@ -2809,7 +2818,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="53"/>
+      <c r="A4" s="56"/>
       <c r="B4" t="s">
         <v>118</v>
       </c>
@@ -2839,7 +2848,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
+      <c r="A5" s="56"/>
       <c r="B5" t="s">
         <v>120</v>
       </c>
@@ -2863,7 +2872,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
+      <c r="A6" s="56"/>
       <c r="B6" t="s">
         <v>122</v>
       </c>
@@ -2890,18 +2899,12 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="53"/>
+      <c r="A7" s="56"/>
       <c r="B7" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="52" t="s">
         <v>156</v>
-      </c>
-      <c r="D7" t="s">
-        <v>150</v>
-      </c>
-      <c r="E7" t="s">
-        <v>195</v>
       </c>
       <c r="F7" s="13" t="s">
         <v>124</v>
@@ -2923,18 +2926,12 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="53"/>
+      <c r="A8" s="56"/>
       <c r="B8" t="s">
         <v>81</v>
       </c>
-      <c r="C8" s="51" t="s">
+      <c r="C8" s="52" t="s">
         <v>157</v>
-      </c>
-      <c r="D8" t="s">
-        <v>150</v>
-      </c>
-      <c r="E8" t="s">
-        <v>195</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>126</v>
@@ -2956,7 +2953,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="53"/>
+      <c r="A9" s="56"/>
       <c r="B9" t="s">
         <v>128</v>
       </c>
@@ -2989,7 +2986,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="53"/>
+      <c r="A10" s="56"/>
       <c r="B10" t="s">
         <v>129</v>
       </c>
@@ -3019,7 +3016,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="53"/>
+      <c r="A11" s="56"/>
       <c r="B11" s="34" t="s">
         <v>131</v>
       </c>
@@ -3035,7 +3032,7 @@
       <c r="K11" s="40"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="53"/>
+      <c r="A12" s="56"/>
       <c r="B12" t="s">
         <v>132</v>
       </c>
@@ -3056,7 +3053,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="53"/>
+      <c r="A13" s="56"/>
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -3086,7 +3083,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="53"/>
+      <c r="A14" s="56"/>
       <c r="B14" s="34" t="s">
         <v>172</v>
       </c>
@@ -3098,7 +3095,7 @@
       <c r="K14" s="40"/>
     </row>
     <row r="15" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="53"/>
+      <c r="A15" s="56"/>
       <c r="B15" s="34" t="s">
         <v>175</v>
       </c>
@@ -3110,7 +3107,7 @@
       <c r="K15" s="40"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="53"/>
+      <c r="A16" s="56"/>
       <c r="B16" t="s">
         <v>133</v>
       </c>
@@ -3137,7 +3134,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="53"/>
+      <c r="A17" s="56"/>
       <c r="B17" t="s">
         <v>136</v>
       </c>
@@ -3164,7 +3161,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="53"/>
+      <c r="A18" s="56"/>
       <c r="B18" t="s">
         <v>139</v>
       </c>
@@ -3188,7 +3185,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="53"/>
+      <c r="A19" s="56"/>
       <c r="B19" t="s">
         <v>140</v>
       </c>
@@ -3218,7 +3215,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="53"/>
+      <c r="A20" s="56"/>
       <c r="B20" t="s">
         <v>27</v>
       </c>
@@ -3248,7 +3245,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="53"/>
+      <c r="A21" s="56"/>
       <c r="B21" t="s">
         <v>55</v>
       </c>
@@ -3278,7 +3275,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="53"/>
+      <c r="A22" s="56"/>
       <c r="B22" t="s">
         <v>74</v>
       </c>
@@ -3308,7 +3305,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="55" t="s">
+      <c r="A23" s="58" t="s">
         <v>141</v>
       </c>
       <c r="B23" s="19" t="s">
@@ -3341,7 +3338,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="56"/>
+      <c r="A24" s="59"/>
       <c r="B24" s="41" t="s">
         <v>5</v>
       </c>
@@ -3368,7 +3365,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="56"/>
+      <c r="A25" s="59"/>
       <c r="B25" s="41" t="s">
         <v>118</v>
       </c>
@@ -3395,7 +3392,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="56"/>
+      <c r="A26" s="59"/>
       <c r="B26" s="41" t="s">
         <v>120</v>
       </c>
@@ -3414,7 +3411,7 @@
       <c r="K26" s="47"/>
     </row>
     <row r="27" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="56"/>
+      <c r="A27" s="59"/>
       <c r="B27" s="41" t="s">
         <v>122</v>
       </c>
@@ -3437,7 +3434,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="56"/>
+      <c r="A28" s="59"/>
       <c r="B28" s="41" t="s">
         <v>128</v>
       </c>
@@ -3464,11 +3461,11 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="56"/>
+      <c r="A29" s="59"/>
       <c r="B29" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="57" t="s">
+      <c r="C29" s="53" t="s">
         <v>171</v>
       </c>
       <c r="D29" s="26" t="s">
@@ -3489,7 +3486,7 @@
       <c r="K29" s="32"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="56"/>
+      <c r="A30" s="59"/>
       <c r="B30" s="26" t="s">
         <v>172</v>
       </c>
@@ -3520,7 +3517,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="56"/>
+      <c r="A31" s="59"/>
       <c r="B31" s="26" t="s">
         <v>175</v>
       </c>
@@ -3551,7 +3548,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="56"/>
+      <c r="A32" s="59"/>
       <c r="B32" s="26" t="s">
         <v>62</v>
       </c>
@@ -3582,7 +3579,7 @@
       </c>
     </row>
     <row r="33" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="56"/>
+      <c r="A33" s="59"/>
       <c r="B33" s="41" t="s">
         <v>67</v>
       </c>
@@ -3609,7 +3606,7 @@
       </c>
     </row>
     <row r="34" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="56"/>
+      <c r="A34" s="59"/>
       <c r="B34" s="41" t="s">
         <v>27</v>
       </c>
@@ -3636,7 +3633,7 @@
       </c>
     </row>
     <row r="35" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="56"/>
+      <c r="A35" s="59"/>
       <c r="B35" s="41" t="s">
         <v>72</v>
       </c>
@@ -3663,7 +3660,7 @@
       </c>
     </row>
     <row r="36" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="56"/>
+      <c r="A36" s="59"/>
       <c r="B36" s="48" t="s">
         <v>74</v>
       </c>
@@ -3690,7 +3687,7 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="55" t="s">
+      <c r="A37" s="58" t="s">
         <v>143</v>
       </c>
       <c r="B37" s="33" t="s">
@@ -3719,7 +3716,7 @@
       </c>
     </row>
     <row r="38" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="56"/>
+      <c r="A38" s="59"/>
       <c r="B38" s="41" t="s">
         <v>118</v>
       </c>
@@ -3746,7 +3743,7 @@
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="56"/>
+      <c r="A39" s="59"/>
       <c r="B39" s="26" t="s">
         <v>79</v>
       </c>
@@ -3776,62 +3773,70 @@
         <v>145</v>
       </c>
     </row>
-    <row r="40" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="56"/>
-      <c r="B40" s="41" t="s">
+    <row r="40" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="59"/>
+      <c r="B40" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="C40" s="41"/>
-      <c r="D40" s="41"/>
-      <c r="E40" s="41"/>
-      <c r="F40" s="42" t="s">
+      <c r="C40" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="D40" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="E40" s="54"/>
+      <c r="F40" s="27" t="s">
         <v>146</v>
       </c>
-      <c r="G40" s="43" t="s">
+      <c r="G40" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="H40" s="44" t="s">
+      <c r="H40" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="I40" s="45" t="s">
+      <c r="I40" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="J40" s="46" t="s">
+      <c r="J40" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="K40" s="47" t="s">
+      <c r="K40" s="32" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="56"/>
-      <c r="B41" s="41" t="s">
+    <row r="41" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="59"/>
+      <c r="B41" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="C41" s="41"/>
-      <c r="D41" s="41"/>
-      <c r="E41" s="41"/>
-      <c r="F41" s="42" t="s">
+      <c r="C41" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D41" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="E41" s="54"/>
+      <c r="F41" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="G41" s="43" t="s">
+      <c r="G41" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="H41" s="44" t="s">
+      <c r="H41" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="I41" s="45" t="s">
+      <c r="I41" s="30" t="s">
         <v>147</v>
       </c>
-      <c r="J41" s="46" t="s">
+      <c r="J41" s="31" t="s">
         <v>147</v>
       </c>
-      <c r="K41" s="47" t="s">
+      <c r="K41" s="32" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="56"/>
+      <c r="A42" s="59"/>
       <c r="B42" s="26" t="s">
         <v>82</v>
       </c>
@@ -3862,7 +3867,7 @@
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="56"/>
+      <c r="A43" s="59"/>
       <c r="B43" s="26" t="s">
         <v>83</v>
       </c>
@@ -3893,7 +3898,7 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="56"/>
+      <c r="A44" s="59"/>
       <c r="B44" s="26" t="s">
         <v>84</v>
       </c>
@@ -3924,7 +3929,7 @@
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="56"/>
+      <c r="A45" s="59"/>
       <c r="B45" s="26" t="s">
         <v>85</v>
       </c>
@@ -3955,7 +3960,7 @@
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="56"/>
+      <c r="A46" s="59"/>
       <c r="B46" s="26" t="s">
         <v>86</v>
       </c>
@@ -3986,7 +3991,7 @@
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="56"/>
+      <c r="A47" s="59"/>
       <c r="B47" s="26" t="s">
         <v>87</v>
       </c>
@@ -4017,7 +4022,7 @@
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="56"/>
+      <c r="A48" s="59"/>
       <c r="B48" s="26" t="s">
         <v>88</v>
       </c>
@@ -4048,7 +4053,7 @@
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="56"/>
+      <c r="A49" s="59"/>
       <c r="B49" s="26" t="s">
         <v>184</v>
       </c>
@@ -4079,7 +4084,7 @@
       </c>
     </row>
     <row r="50" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="56"/>
+      <c r="A50" s="59"/>
       <c r="B50" s="41" t="s">
         <v>89</v>
       </c>
@@ -4106,7 +4111,7 @@
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="56"/>
+      <c r="A51" s="59"/>
       <c r="B51" s="26" t="s">
         <v>90</v>
       </c>
@@ -4137,7 +4142,7 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="56"/>
+      <c r="A52" s="59"/>
       <c r="B52" s="26" t="s">
         <v>91</v>
       </c>
@@ -4168,7 +4173,7 @@
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="56"/>
+      <c r="A53" s="59"/>
       <c r="B53" s="26" t="s">
         <v>92</v>
       </c>
@@ -4199,7 +4204,7 @@
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="56"/>
+      <c r="A54" s="59"/>
       <c r="B54" s="26" t="s">
         <v>93</v>
       </c>
@@ -4230,7 +4235,7 @@
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="56"/>
+      <c r="A55" s="59"/>
       <c r="B55" s="26" t="s">
         <v>94</v>
       </c>

</xml_diff>